<commit_message>
add land normalization factors to xslx
</commit_message>
<xml_diff>
--- a/Studies/USMap_Doubleday_2024/SETUPS Description Complete_sil.xlsx
+++ b/Studies/USMap_Doubleday_2024/SETUPS Description Complete_sil.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sayala\Documents\GitHub\InSPIRE\Studies\USMap_Doubleday_2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tford\dev\InSPIRE\Studies\USMap_Doubleday_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3D56A2-4FE6-47DD-88B8-0922CC8F8D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F15CF2-F669-4E73-B140-F4D48BF3E42B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720" xr2:uid="{20F8F7F2-6405-4778-91BF-D0B7AC5935BA}"/>
+    <workbookView xWindow="28680" yWindow="-4470" windowWidth="16440" windowHeight="28320" xr2:uid="{20F8F7F2-6405-4778-91BF-D0B7AC5935BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="115">
   <si>
     <t>Scenario</t>
   </si>
@@ -441,6 +441,45 @@
   <si>
     <t>Varying, …</t>
   </si>
+  <si>
+    <t>Calculated in SAM's Land Area Estimate with 1.0 land area multiplier and 0 additional land area</t>
+  </si>
+  <si>
+    <t>Ground area= total module area/GCR = total module area/(collector width/pitch) = total module area * pitch/collector width</t>
+  </si>
+  <si>
+    <t>Setup</t>
+  </si>
+  <si>
+    <t>kWdc</t>
+  </si>
+  <si>
+    <t>Collector width (m)</t>
+  </si>
+  <si>
+    <t>Pitch (m)</t>
+  </si>
+  <si>
+    <t>Total module area (acres)</t>
+  </si>
+  <si>
+    <t>Ground area occupied by array (acres)</t>
+  </si>
+  <si>
+    <t>Doubling ground area to account for panel tiling</t>
+  </si>
+  <si>
+    <t>Eqn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Double-check by calculating ground area: </t>
+  </si>
+  <si>
+    <t>variable (tonita)</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
 </sst>
 </file>
 
@@ -449,7 +488,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -555,6 +594,35 @@
       <b/>
       <sz val="8"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -814,7 +882,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -937,66 +1005,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1004,6 +1017,76 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1036,8 +1119,8 @@
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>752</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>543677</xdr:colOff>
       <xdr:row>74</xdr:row>
       <xdr:rowOff>105034</xdr:rowOff>
     </xdr:to>
@@ -1424,10 +1507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932A1107-9899-4DFE-A9E6-0ED2844D3F4A}">
-  <dimension ref="B2:AA90"/>
+  <dimension ref="B2:AA108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+    <sheetView tabSelected="1" topLeftCell="B61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H83" sqref="H83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1438,7 +1521,7 @@
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" customWidth="1"/>
     <col min="7" max="7" width="20.42578125" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="25.5703125" customWidth="1"/>
     <col min="9" max="9" width="18.7109375" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
     <col min="15" max="15" width="13.28515625" style="1" customWidth="1"/>
@@ -1451,10 +1534,10 @@
       <c r="B2" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="T2" s="73" t="s">
+      <c r="T2" s="75" t="s">
         <v>60</v>
       </c>
-      <c r="U2" s="73"/>
+      <c r="U2" s="75"/>
     </row>
     <row r="3" spans="2:21" ht="53.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="24" t="s">
@@ -1506,7 +1589,7 @@
       <c r="R3" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="S3" s="86" t="s">
+      <c r="S3" s="67" t="s">
         <v>92</v>
       </c>
       <c r="T3" s="25" t="s">
@@ -1776,7 +1859,7 @@
       <c r="T8" s="28"/>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B9" s="84" t="s">
+      <c r="B9" s="65" t="s">
         <v>96</v>
       </c>
       <c r="C9">
@@ -2264,11 +2347,11 @@
       <c r="D27" s="13"/>
       <c r="E27" s="13"/>
       <c r="F27" s="14"/>
-      <c r="G27" s="74" t="s">
+      <c r="G27" s="76" t="s">
         <v>39</v>
       </c>
-      <c r="H27" s="75"/>
-      <c r="I27" s="75"/>
+      <c r="H27" s="77"/>
+      <c r="I27" s="77"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
@@ -2278,9 +2361,9 @@
         <v>8</v>
       </c>
       <c r="F28" s="6"/>
-      <c r="G28" s="76"/>
-      <c r="H28" s="67"/>
-      <c r="I28" s="67"/>
+      <c r="G28" s="78"/>
+      <c r="H28" s="79"/>
+      <c r="I28" s="79"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
@@ -2290,9 +2373,9 @@
         <v>2</v>
       </c>
       <c r="F29" s="6"/>
-      <c r="G29" s="76"/>
-      <c r="H29" s="67"/>
-      <c r="I29" s="67"/>
+      <c r="G29" s="78"/>
+      <c r="H29" s="79"/>
+      <c r="I29" s="79"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
@@ -2310,9 +2393,9 @@
       <c r="F30" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G30" s="76"/>
-      <c r="H30" s="67"/>
-      <c r="I30" s="67"/>
+      <c r="G30" s="78"/>
+      <c r="H30" s="79"/>
+      <c r="I30" s="79"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
@@ -2334,11 +2417,11 @@
         <f>ROUND(D31/10,0)</f>
         <v>3</v>
       </c>
-      <c r="G31" s="68" t="s">
+      <c r="G31" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="H31" s="69"/>
-      <c r="I31" s="69"/>
+      <c r="H31" s="74"/>
+      <c r="I31" s="74"/>
     </row>
     <row r="32" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="9" t="s">
@@ -2360,46 +2443,46 @@
         <f>ROUND(D32/10,0)</f>
         <v>8</v>
       </c>
-      <c r="G32" s="68" t="s">
+      <c r="G32" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="H32" s="69"/>
-      <c r="I32" s="69"/>
+      <c r="H32" s="74"/>
+      <c r="I32" s="74"/>
     </row>
     <row r="36" spans="3:26" x14ac:dyDescent="0.25">
       <c r="O36"/>
     </row>
     <row r="37" spans="3:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="62"/>
+      <c r="C37" s="81"/>
       <c r="D37" s="36"/>
       <c r="E37" s="36"/>
-      <c r="F37" s="77" t="s">
+      <c r="F37" s="80" t="s">
         <v>59</v>
       </c>
-      <c r="G37" s="77"/>
-      <c r="H37" s="77"/>
-      <c r="I37" s="77"/>
-      <c r="J37" s="62" t="s">
+      <c r="G37" s="80"/>
+      <c r="H37" s="80"/>
+      <c r="I37" s="80"/>
+      <c r="J37" s="81" t="s">
         <v>58</v>
       </c>
-      <c r="K37" s="62"/>
-      <c r="L37" s="62"/>
-      <c r="M37" s="62"/>
-      <c r="N37" s="62"/>
-      <c r="O37" s="62"/>
-      <c r="P37" s="62"/>
-      <c r="Q37" s="62"/>
-      <c r="R37" s="62"/>
-      <c r="S37" s="62"/>
-      <c r="T37" s="62"/>
-      <c r="U37" s="62"/>
-      <c r="V37" s="62"/>
-      <c r="W37" s="62"/>
-      <c r="X37" s="62"/>
-      <c r="Y37" s="62"/>
+      <c r="K37" s="81"/>
+      <c r="L37" s="81"/>
+      <c r="M37" s="81"/>
+      <c r="N37" s="81"/>
+      <c r="O37" s="81"/>
+      <c r="P37" s="81"/>
+      <c r="Q37" s="81"/>
+      <c r="R37" s="81"/>
+      <c r="S37" s="81"/>
+      <c r="T37" s="81"/>
+      <c r="U37" s="81"/>
+      <c r="V37" s="81"/>
+      <c r="W37" s="81"/>
+      <c r="X37" s="81"/>
+      <c r="Y37" s="81"/>
     </row>
     <row r="38" spans="3:26" s="37" customFormat="1" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C38" s="62"/>
+      <c r="C38" s="81"/>
       <c r="D38" s="38" t="s">
         <v>0</v>
       </c>
@@ -2466,12 +2549,12 @@
       <c r="Y38" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="Z38" s="78" t="s">
+      <c r="Z38" s="62" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="39" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C39" s="63" t="s">
+      <c r="C39" s="82" t="s">
         <v>66</v>
       </c>
       <c r="D39">
@@ -2524,7 +2607,7 @@
       </c>
     </row>
     <row r="40" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C40" s="63"/>
+      <c r="C40" s="82"/>
       <c r="D40">
         <v>2</v>
       </c>
@@ -2575,7 +2658,7 @@
       </c>
     </row>
     <row r="41" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C41" s="63"/>
+      <c r="C41" s="82"/>
       <c r="D41">
         <v>3</v>
       </c>
@@ -2626,7 +2709,7 @@
       </c>
     </row>
     <row r="42" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C42" s="63"/>
+      <c r="C42" s="82"/>
       <c r="D42">
         <v>4</v>
       </c>
@@ -2677,7 +2760,7 @@
       </c>
     </row>
     <row r="43" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C43" s="63"/>
+      <c r="C43" s="82"/>
       <c r="D43">
         <v>5</v>
       </c>
@@ -2832,39 +2915,39 @@
       <c r="M48" s="1"/>
       <c r="O48"/>
     </row>
-    <row r="49" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C49" s="64" t="s">
+    <row r="49" spans="3:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C49" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="D49" s="66" t="s">
+      <c r="D49" s="85" t="s">
         <v>62</v>
       </c>
-      <c r="E49" s="66"/>
-      <c r="F49" s="77" t="s">
+      <c r="E49" s="85"/>
+      <c r="F49" s="80" t="s">
         <v>59</v>
       </c>
-      <c r="G49" s="77"/>
-      <c r="H49" s="77"/>
-      <c r="I49" s="77"/>
-      <c r="J49" s="62" t="s">
+      <c r="G49" s="80"/>
+      <c r="H49" s="80"/>
+      <c r="I49" s="80"/>
+      <c r="J49" s="81" t="s">
         <v>58</v>
       </c>
-      <c r="K49" s="62"/>
-      <c r="L49" s="62"/>
-      <c r="M49" s="62"/>
-      <c r="N49" s="62"/>
-      <c r="O49" s="62"/>
-      <c r="P49" s="62"/>
-      <c r="Q49" s="62"/>
-      <c r="R49" s="62"/>
-      <c r="S49" s="62"/>
+      <c r="K49" s="81"/>
+      <c r="L49" s="81"/>
+      <c r="M49" s="81"/>
+      <c r="N49" s="81"/>
+      <c r="O49" s="81"/>
+      <c r="P49" s="81"/>
+      <c r="Q49" s="81"/>
+      <c r="R49" s="81"/>
+      <c r="S49" s="81"/>
     </row>
     <row r="50" spans="3:19" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C50" s="64"/>
-      <c r="D50" s="65" t="s">
+      <c r="C50" s="83"/>
+      <c r="D50" s="84" t="s">
         <v>63</v>
       </c>
-      <c r="E50" s="65"/>
+      <c r="E50" s="84"/>
       <c r="F50" s="39" t="s">
         <v>57</v>
       </c>
@@ -2909,11 +2992,11 @@
       </c>
     </row>
     <row r="51" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C51" s="64"/>
-      <c r="D51" s="67">
+      <c r="C51" s="83"/>
+      <c r="D51" s="79">
         <v>3.8</v>
       </c>
-      <c r="E51" s="67"/>
+      <c r="E51" s="79"/>
       <c r="F51">
         <v>0</v>
       </c>
@@ -2958,11 +3041,11 @@
       </c>
     </row>
     <row r="52" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C52" s="64"/>
-      <c r="D52" s="67">
+      <c r="C52" s="83"/>
+      <c r="D52" s="79">
         <v>4</v>
       </c>
-      <c r="E52" s="67"/>
+      <c r="E52" s="79"/>
       <c r="F52">
         <v>0</v>
       </c>
@@ -3007,11 +3090,11 @@
       </c>
     </row>
     <row r="53" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C53" s="64"/>
-      <c r="D53" s="67">
+      <c r="C53" s="83"/>
+      <c r="D53" s="79">
         <v>4.5</v>
       </c>
-      <c r="E53" s="67"/>
+      <c r="E53" s="79"/>
       <c r="F53">
         <v>0</v>
       </c>
@@ -3056,11 +3139,11 @@
       </c>
     </row>
     <row r="54" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C54" s="64"/>
-      <c r="D54" s="67">
+      <c r="C54" s="83"/>
+      <c r="D54" s="79">
         <v>5</v>
       </c>
-      <c r="E54" s="67"/>
+      <c r="E54" s="79"/>
       <c r="F54">
         <v>0</v>
       </c>
@@ -3105,11 +3188,11 @@
       </c>
     </row>
     <row r="55" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C55" s="64"/>
-      <c r="D55" s="67">
+      <c r="C55" s="83"/>
+      <c r="D55" s="79">
         <v>5.5</v>
       </c>
-      <c r="E55" s="67"/>
+      <c r="E55" s="79"/>
       <c r="F55">
         <v>0</v>
       </c>
@@ -3154,11 +3237,11 @@
       </c>
     </row>
     <row r="56" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C56" s="64"/>
-      <c r="D56" s="67">
+      <c r="C56" s="83"/>
+      <c r="D56" s="79">
         <v>6</v>
       </c>
-      <c r="E56" s="67"/>
+      <c r="E56" s="79"/>
       <c r="F56">
         <v>0</v>
       </c>
@@ -3203,11 +3286,11 @@
       </c>
     </row>
     <row r="57" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C57" s="64"/>
-      <c r="D57" s="67">
+      <c r="C57" s="83"/>
+      <c r="D57" s="79">
         <v>6.5</v>
       </c>
-      <c r="E57" s="67"/>
+      <c r="E57" s="79"/>
       <c r="F57">
         <v>0</v>
       </c>
@@ -3252,11 +3335,11 @@
       </c>
     </row>
     <row r="58" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C58" s="64"/>
-      <c r="D58" s="67">
+      <c r="C58" s="83"/>
+      <c r="D58" s="79">
         <v>7</v>
       </c>
-      <c r="E58" s="67"/>
+      <c r="E58" s="79"/>
       <c r="F58">
         <v>0</v>
       </c>
@@ -3301,11 +3384,11 @@
       </c>
     </row>
     <row r="59" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C59" s="64"/>
-      <c r="D59" s="67">
+      <c r="C59" s="83"/>
+      <c r="D59" s="79">
         <v>7.5</v>
       </c>
-      <c r="E59" s="67"/>
+      <c r="E59" s="79"/>
       <c r="F59">
         <v>0</v>
       </c>
@@ -3350,11 +3433,11 @@
       </c>
     </row>
     <row r="60" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C60" s="64"/>
-      <c r="D60" s="67">
+      <c r="C60" s="83"/>
+      <c r="D60" s="79">
         <v>8</v>
       </c>
-      <c r="E60" s="67"/>
+      <c r="E60" s="79"/>
       <c r="F60">
         <v>0</v>
       </c>
@@ -3399,11 +3482,11 @@
       </c>
     </row>
     <row r="61" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C61" s="64"/>
-      <c r="D61" s="67">
+      <c r="C61" s="83"/>
+      <c r="D61" s="79">
         <v>8.5</v>
       </c>
-      <c r="E61" s="67"/>
+      <c r="E61" s="79"/>
       <c r="F61">
         <v>0</v>
       </c>
@@ -3448,11 +3531,11 @@
       </c>
     </row>
     <row r="62" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C62" s="64"/>
-      <c r="D62" s="67">
+      <c r="C62" s="83"/>
+      <c r="D62" s="79">
         <v>9</v>
       </c>
-      <c r="E62" s="67"/>
+      <c r="E62" s="79"/>
       <c r="F62">
         <v>0</v>
       </c>
@@ -3565,10 +3648,10 @@
         <v>73</v>
       </c>
       <c r="E67" s="59"/>
-      <c r="F67" s="82" t="s">
+      <c r="F67" s="68" t="s">
         <v>95</v>
       </c>
-      <c r="G67" s="83"/>
+      <c r="G67" s="69"/>
     </row>
     <row r="68" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C68" s="5" t="s">
@@ -3581,10 +3664,10 @@
       <c r="E68" s="59" t="s">
         <v>74</v>
       </c>
-      <c r="F68" s="80">
+      <c r="F68" s="63">
         <v>0.5</v>
       </c>
-      <c r="G68" s="81" t="s">
+      <c r="G68" s="64" t="s">
         <v>71</v>
       </c>
     </row>
@@ -3680,12 +3763,12 @@
       </c>
     </row>
     <row r="77" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="C77" s="79" t="s">
+      <c r="C77" s="5" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="78" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="C78" s="79" t="s">
+      <c r="C78" s="5" t="s">
         <v>94</v>
       </c>
     </row>
@@ -3697,28 +3780,28 @@
       <c r="D80" s="71"/>
       <c r="E80" s="72"/>
     </row>
-    <row r="81" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="3:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C81" s="9" t="s">
         <v>84</v>
       </c>
       <c r="D81" s="58" t="s">
         <v>85</v>
       </c>
-      <c r="E81" s="85" t="s">
+      <c r="E81" s="66" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="83" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C83" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="84" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C84" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="85" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C85" t="s">
         <v>87</v>
       </c>
@@ -3726,15 +3809,15 @@
         <v>83</v>
       </c>
     </row>
-    <row r="87" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="88" spans="3:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="88" spans="3:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C88" s="70" t="s">
         <v>99</v>
       </c>
       <c r="D88" s="71"/>
       <c r="E88" s="72"/>
     </row>
-    <row r="89" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C89" s="2"/>
       <c r="D89" s="3" t="s">
         <v>97</v>
@@ -3744,32 +3827,306 @@
         <v>100</v>
       </c>
     </row>
-    <row r="90" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C90" s="9"/>
       <c r="D90" s="58" t="s">
         <v>98</v>
       </c>
       <c r="E90" s="11"/>
     </row>
+    <row r="95" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="96" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C96" s="87" t="s">
+        <v>102</v>
+      </c>
+      <c r="D96" s="88"/>
+      <c r="E96" s="88"/>
+      <c r="F96" s="88"/>
+      <c r="G96" s="88"/>
+      <c r="H96" s="89"/>
+      <c r="I96" s="90"/>
+      <c r="J96" s="86"/>
+    </row>
+    <row r="97" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C97" s="91" t="s">
+        <v>103</v>
+      </c>
+      <c r="D97" s="92"/>
+      <c r="E97" s="92"/>
+      <c r="F97" s="92"/>
+      <c r="G97" s="92"/>
+      <c r="H97" s="92"/>
+      <c r="I97" s="93"/>
+      <c r="J97" s="86"/>
+    </row>
+    <row r="98" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C98" s="94" t="s">
+        <v>104</v>
+      </c>
+      <c r="D98" s="95" t="s">
+        <v>105</v>
+      </c>
+      <c r="E98" s="95" t="s">
+        <v>106</v>
+      </c>
+      <c r="F98" s="95" t="s">
+        <v>107</v>
+      </c>
+      <c r="G98" s="95" t="s">
+        <v>17</v>
+      </c>
+      <c r="H98" s="95" t="s">
+        <v>108</v>
+      </c>
+      <c r="I98" s="96" t="s">
+        <v>109</v>
+      </c>
+      <c r="J98" s="86"/>
+    </row>
+    <row r="99" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C99" s="94">
+        <v>1</v>
+      </c>
+      <c r="D99" s="95">
+        <v>80.066000000000003</v>
+      </c>
+      <c r="E99" s="95">
+        <v>2</v>
+      </c>
+      <c r="F99" s="95">
+        <v>5</v>
+      </c>
+      <c r="G99" s="95">
+        <v>0.4</v>
+      </c>
+      <c r="H99" s="95">
+        <v>0.104</v>
+      </c>
+      <c r="I99" s="96">
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="J99" s="86"/>
+    </row>
+    <row r="100" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C100" s="94">
+        <v>2</v>
+      </c>
+      <c r="D100" s="95">
+        <v>80.066000000000003</v>
+      </c>
+      <c r="E100" s="95">
+        <v>2</v>
+      </c>
+      <c r="F100" s="95">
+        <v>5</v>
+      </c>
+      <c r="G100" s="95">
+        <v>0.4</v>
+      </c>
+      <c r="H100" s="95">
+        <v>0.104</v>
+      </c>
+      <c r="I100" s="96">
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="J100" s="86"/>
+    </row>
+    <row r="101" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C101" s="94">
+        <v>3</v>
+      </c>
+      <c r="D101" s="95">
+        <v>80.066000000000003</v>
+      </c>
+      <c r="E101" s="95">
+        <v>2</v>
+      </c>
+      <c r="F101" s="95">
+        <v>5</v>
+      </c>
+      <c r="G101" s="95">
+        <v>0.2</v>
+      </c>
+      <c r="H101" s="95">
+        <v>0.104</v>
+      </c>
+      <c r="I101" s="96">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="J101" s="86" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="102" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C102" s="94">
+        <v>4</v>
+      </c>
+      <c r="D102" s="95">
+        <v>80.066000000000003</v>
+      </c>
+      <c r="E102" s="95">
+        <v>2</v>
+      </c>
+      <c r="F102" s="95">
+        <v>8</v>
+      </c>
+      <c r="G102" s="95">
+        <v>0.25</v>
+      </c>
+      <c r="H102" s="95">
+        <v>0.104</v>
+      </c>
+      <c r="I102" s="96">
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="J102" s="86"/>
+    </row>
+    <row r="103" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C103" s="94">
+        <v>5</v>
+      </c>
+      <c r="D103" s="95">
+        <v>80.066000000000003</v>
+      </c>
+      <c r="E103" s="95">
+        <v>2</v>
+      </c>
+      <c r="F103" s="95">
+        <v>11</v>
+      </c>
+      <c r="G103" s="95">
+        <v>0.18181818199999999</v>
+      </c>
+      <c r="H103" s="95">
+        <v>0.104</v>
+      </c>
+      <c r="I103" s="96">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="J103" s="86"/>
+    </row>
+    <row r="104" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C104" s="97">
+        <v>6</v>
+      </c>
+      <c r="D104" s="92">
+        <v>80.066000000000003</v>
+      </c>
+      <c r="E104" s="92">
+        <v>2</v>
+      </c>
+      <c r="F104" s="92" t="s">
+        <v>114</v>
+      </c>
+      <c r="G104" s="92" t="s">
+        <v>113</v>
+      </c>
+      <c r="H104" s="92">
+        <v>0.104</v>
+      </c>
+      <c r="I104" s="98" t="s">
+        <v>111</v>
+      </c>
+      <c r="J104" s="86"/>
+    </row>
+    <row r="105" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C105" s="97">
+        <v>7</v>
+      </c>
+      <c r="D105" s="92">
+        <v>80.066000000000003</v>
+      </c>
+      <c r="E105" s="92">
+        <v>2</v>
+      </c>
+      <c r="F105" s="92" t="s">
+        <v>114</v>
+      </c>
+      <c r="G105" s="92" t="s">
+        <v>113</v>
+      </c>
+      <c r="H105" s="92">
+        <v>0.104</v>
+      </c>
+      <c r="I105" s="98" t="s">
+        <v>111</v>
+      </c>
+      <c r="J105" s="86"/>
+    </row>
+    <row r="106" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C106" s="97">
+        <v>8</v>
+      </c>
+      <c r="D106" s="92">
+        <v>80.066000000000003</v>
+      </c>
+      <c r="E106" s="92">
+        <v>2</v>
+      </c>
+      <c r="F106" s="92" t="s">
+        <v>114</v>
+      </c>
+      <c r="G106" s="92" t="s">
+        <v>113</v>
+      </c>
+      <c r="H106" s="92">
+        <v>0.104</v>
+      </c>
+      <c r="I106" s="98" t="s">
+        <v>111</v>
+      </c>
+      <c r="J106" s="86"/>
+    </row>
+    <row r="107" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C107" s="97">
+        <v>9</v>
+      </c>
+      <c r="D107" s="92">
+        <v>80.066000000000003</v>
+      </c>
+      <c r="E107" s="92">
+        <v>2</v>
+      </c>
+      <c r="F107" s="92" t="s">
+        <v>114</v>
+      </c>
+      <c r="G107" s="92" t="s">
+        <v>113</v>
+      </c>
+      <c r="H107" s="92">
+        <v>0.104</v>
+      </c>
+      <c r="I107" s="98" t="s">
+        <v>111</v>
+      </c>
+      <c r="J107" s="86"/>
+    </row>
+    <row r="108" spans="3:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C108" s="99">
+        <v>10</v>
+      </c>
+      <c r="D108" s="100">
+        <v>80.066000000000003</v>
+      </c>
+      <c r="E108" s="100">
+        <v>2</v>
+      </c>
+      <c r="F108" s="100">
+        <v>8.6</v>
+      </c>
+      <c r="G108" s="100"/>
+      <c r="H108" s="100">
+        <v>0.104</v>
+      </c>
+      <c r="I108" s="101">
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="J108" s="86" t="s">
+        <v>112</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="C88:E88"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="C80:E80"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="F49:I49"/>
     <mergeCell ref="J37:Y37"/>
     <mergeCell ref="J49:S49"/>
     <mergeCell ref="C39:C43"/>
@@ -3784,6 +4141,23 @@
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="D59:E59"/>
     <mergeCell ref="D60:E60"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="C88:E88"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="C80:E80"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="F49:I49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Add power normalization factors
</commit_message>
<xml_diff>
--- a/Studies/USMap_Doubleday_2024/SETUPS Description Complete_sil.xlsx
+++ b/Studies/USMap_Doubleday_2024/SETUPS Description Complete_sil.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tford\dev\InSPIRE\Studies\USMap_Doubleday_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F15CF2-F669-4E73-B140-F4D48BF3E42B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1A2BFF-A824-4EBB-BF2E-3EFAB88E3E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-4470" windowWidth="16440" windowHeight="28320" xr2:uid="{20F8F7F2-6405-4778-91BF-D0B7AC5935BA}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -94,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="112">
   <si>
     <t>Scenario</t>
   </si>
@@ -427,16 +428,7 @@
     <t>5.5 PENDING</t>
   </si>
   <si>
-    <t>per Land Area</t>
-  </si>
-  <si>
-    <t>per kWdc installed</t>
-  </si>
-  <si>
     <t>Power Calculation Normalizaiton Factor</t>
-  </si>
-  <si>
-    <t>&lt;- if expaded for system to cover an acre, what installed capacity be (function of the pitch)</t>
   </si>
   <si>
     <t>Varying, …</t>
@@ -882,7 +874,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1017,76 +1009,75 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1509,8 +1500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932A1107-9899-4DFE-A9E6-0ED2844D3F4A}">
   <dimension ref="B2:AA108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H83" sqref="H83"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J92" sqref="J92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1534,12 +1525,12 @@
       <c r="B2" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="T2" s="75" t="s">
+      <c r="T2" s="89" t="s">
         <v>60</v>
       </c>
-      <c r="U2" s="75"/>
-    </row>
-    <row r="3" spans="2:21" ht="53.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U2" s="89"/>
+    </row>
+    <row r="3" spans="2:21" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="24" t="s">
         <v>0</v>
       </c>
@@ -1922,7 +1913,7 @@
         <v>20</v>
       </c>
       <c r="S10" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="T10" s="28"/>
       <c r="U10" s="20"/>
@@ -1977,7 +1968,7 @@
         <v>20</v>
       </c>
       <c r="S11" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="T11" s="28"/>
       <c r="U11" s="20"/>
@@ -2032,7 +2023,7 @@
         <v>20</v>
       </c>
       <c r="S12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="T12" s="28"/>
       <c r="U12" s="20"/>
@@ -2087,7 +2078,7 @@
         <v>20</v>
       </c>
       <c r="S13" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="T13" s="28"/>
       <c r="U13" s="20"/>
@@ -2347,11 +2338,11 @@
       <c r="D27" s="13"/>
       <c r="E27" s="13"/>
       <c r="F27" s="14"/>
-      <c r="G27" s="76" t="s">
+      <c r="G27" s="90" t="s">
         <v>39</v>
       </c>
-      <c r="H27" s="77"/>
-      <c r="I27" s="77"/>
+      <c r="H27" s="91"/>
+      <c r="I27" s="91"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
@@ -2361,9 +2352,9 @@
         <v>8</v>
       </c>
       <c r="F28" s="6"/>
-      <c r="G28" s="78"/>
-      <c r="H28" s="79"/>
-      <c r="I28" s="79"/>
+      <c r="G28" s="92"/>
+      <c r="H28" s="88"/>
+      <c r="I28" s="88"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
@@ -2373,9 +2364,9 @@
         <v>2</v>
       </c>
       <c r="F29" s="6"/>
-      <c r="G29" s="78"/>
-      <c r="H29" s="79"/>
-      <c r="I29" s="79"/>
+      <c r="G29" s="92"/>
+      <c r="H29" s="88"/>
+      <c r="I29" s="88"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
@@ -2393,9 +2384,9 @@
       <c r="F30" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G30" s="78"/>
-      <c r="H30" s="79"/>
-      <c r="I30" s="79"/>
+      <c r="G30" s="92"/>
+      <c r="H30" s="88"/>
+      <c r="I30" s="88"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
@@ -2417,11 +2408,11 @@
         <f>ROUND(D31/10,0)</f>
         <v>3</v>
       </c>
-      <c r="G31" s="73" t="s">
+      <c r="G31" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="H31" s="74"/>
-      <c r="I31" s="74"/>
+      <c r="H31" s="99"/>
+      <c r="I31" s="99"/>
     </row>
     <row r="32" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="9" t="s">
@@ -2443,46 +2434,46 @@
         <f>ROUND(D32/10,0)</f>
         <v>8</v>
       </c>
-      <c r="G32" s="73" t="s">
+      <c r="G32" s="98" t="s">
         <v>38</v>
       </c>
-      <c r="H32" s="74"/>
-      <c r="I32" s="74"/>
+      <c r="H32" s="99"/>
+      <c r="I32" s="99"/>
     </row>
     <row r="36" spans="3:26" x14ac:dyDescent="0.25">
       <c r="O36"/>
     </row>
     <row r="37" spans="3:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="81"/>
+      <c r="C37" s="83"/>
       <c r="D37" s="36"/>
       <c r="E37" s="36"/>
-      <c r="F37" s="80" t="s">
+      <c r="F37" s="100" t="s">
         <v>59</v>
       </c>
-      <c r="G37" s="80"/>
-      <c r="H37" s="80"/>
-      <c r="I37" s="80"/>
-      <c r="J37" s="81" t="s">
+      <c r="G37" s="100"/>
+      <c r="H37" s="100"/>
+      <c r="I37" s="100"/>
+      <c r="J37" s="83" t="s">
         <v>58</v>
       </c>
-      <c r="K37" s="81"/>
-      <c r="L37" s="81"/>
-      <c r="M37" s="81"/>
-      <c r="N37" s="81"/>
-      <c r="O37" s="81"/>
-      <c r="P37" s="81"/>
-      <c r="Q37" s="81"/>
-      <c r="R37" s="81"/>
-      <c r="S37" s="81"/>
-      <c r="T37" s="81"/>
-      <c r="U37" s="81"/>
-      <c r="V37" s="81"/>
-      <c r="W37" s="81"/>
-      <c r="X37" s="81"/>
-      <c r="Y37" s="81"/>
+      <c r="K37" s="83"/>
+      <c r="L37" s="83"/>
+      <c r="M37" s="83"/>
+      <c r="N37" s="83"/>
+      <c r="O37" s="83"/>
+      <c r="P37" s="83"/>
+      <c r="Q37" s="83"/>
+      <c r="R37" s="83"/>
+      <c r="S37" s="83"/>
+      <c r="T37" s="83"/>
+      <c r="U37" s="83"/>
+      <c r="V37" s="83"/>
+      <c r="W37" s="83"/>
+      <c r="X37" s="83"/>
+      <c r="Y37" s="83"/>
     </row>
     <row r="38" spans="3:26" s="37" customFormat="1" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C38" s="81"/>
+      <c r="C38" s="83"/>
       <c r="D38" s="38" t="s">
         <v>0</v>
       </c>
@@ -2554,7 +2545,7 @@
       </c>
     </row>
     <row r="39" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C39" s="82" t="s">
+      <c r="C39" s="84" t="s">
         <v>66</v>
       </c>
       <c r="D39">
@@ -2607,7 +2598,7 @@
       </c>
     </row>
     <row r="40" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C40" s="82"/>
+      <c r="C40" s="84"/>
       <c r="D40">
         <v>2</v>
       </c>
@@ -2658,7 +2649,7 @@
       </c>
     </row>
     <row r="41" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C41" s="82"/>
+      <c r="C41" s="84"/>
       <c r="D41">
         <v>3</v>
       </c>
@@ -2709,7 +2700,7 @@
       </c>
     </row>
     <row r="42" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C42" s="82"/>
+      <c r="C42" s="84"/>
       <c r="D42">
         <v>4</v>
       </c>
@@ -2760,7 +2751,7 @@
       </c>
     </row>
     <row r="43" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C43" s="82"/>
+      <c r="C43" s="84"/>
       <c r="D43">
         <v>5</v>
       </c>
@@ -2916,38 +2907,38 @@
       <c r="O48"/>
     </row>
     <row r="49" spans="3:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C49" s="83" t="s">
+      <c r="C49" s="85" t="s">
         <v>68</v>
       </c>
-      <c r="D49" s="85" t="s">
+      <c r="D49" s="87" t="s">
         <v>62</v>
       </c>
-      <c r="E49" s="85"/>
-      <c r="F49" s="80" t="s">
+      <c r="E49" s="87"/>
+      <c r="F49" s="100" t="s">
         <v>59</v>
       </c>
-      <c r="G49" s="80"/>
-      <c r="H49" s="80"/>
-      <c r="I49" s="80"/>
-      <c r="J49" s="81" t="s">
+      <c r="G49" s="100"/>
+      <c r="H49" s="100"/>
+      <c r="I49" s="100"/>
+      <c r="J49" s="83" t="s">
         <v>58</v>
       </c>
-      <c r="K49" s="81"/>
-      <c r="L49" s="81"/>
-      <c r="M49" s="81"/>
-      <c r="N49" s="81"/>
-      <c r="O49" s="81"/>
-      <c r="P49" s="81"/>
-      <c r="Q49" s="81"/>
-      <c r="R49" s="81"/>
-      <c r="S49" s="81"/>
+      <c r="K49" s="83"/>
+      <c r="L49" s="83"/>
+      <c r="M49" s="83"/>
+      <c r="N49" s="83"/>
+      <c r="O49" s="83"/>
+      <c r="P49" s="83"/>
+      <c r="Q49" s="83"/>
+      <c r="R49" s="83"/>
+      <c r="S49" s="83"/>
     </row>
     <row r="50" spans="3:19" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C50" s="83"/>
-      <c r="D50" s="84" t="s">
+      <c r="C50" s="85"/>
+      <c r="D50" s="86" t="s">
         <v>63</v>
       </c>
-      <c r="E50" s="84"/>
+      <c r="E50" s="86"/>
       <c r="F50" s="39" t="s">
         <v>57</v>
       </c>
@@ -2992,11 +2983,11 @@
       </c>
     </row>
     <row r="51" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C51" s="83"/>
-      <c r="D51" s="79">
+      <c r="C51" s="85"/>
+      <c r="D51" s="88">
         <v>3.8</v>
       </c>
-      <c r="E51" s="79"/>
+      <c r="E51" s="88"/>
       <c r="F51">
         <v>0</v>
       </c>
@@ -3041,11 +3032,11 @@
       </c>
     </row>
     <row r="52" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C52" s="83"/>
-      <c r="D52" s="79">
+      <c r="C52" s="85"/>
+      <c r="D52" s="88">
         <v>4</v>
       </c>
-      <c r="E52" s="79"/>
+      <c r="E52" s="88"/>
       <c r="F52">
         <v>0</v>
       </c>
@@ -3090,11 +3081,11 @@
       </c>
     </row>
     <row r="53" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C53" s="83"/>
-      <c r="D53" s="79">
+      <c r="C53" s="85"/>
+      <c r="D53" s="88">
         <v>4.5</v>
       </c>
-      <c r="E53" s="79"/>
+      <c r="E53" s="88"/>
       <c r="F53">
         <v>0</v>
       </c>
@@ -3139,11 +3130,11 @@
       </c>
     </row>
     <row r="54" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C54" s="83"/>
-      <c r="D54" s="79">
+      <c r="C54" s="85"/>
+      <c r="D54" s="88">
         <v>5</v>
       </c>
-      <c r="E54" s="79"/>
+      <c r="E54" s="88"/>
       <c r="F54">
         <v>0</v>
       </c>
@@ -3188,11 +3179,11 @@
       </c>
     </row>
     <row r="55" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C55" s="83"/>
-      <c r="D55" s="79">
+      <c r="C55" s="85"/>
+      <c r="D55" s="88">
         <v>5.5</v>
       </c>
-      <c r="E55" s="79"/>
+      <c r="E55" s="88"/>
       <c r="F55">
         <v>0</v>
       </c>
@@ -3237,11 +3228,11 @@
       </c>
     </row>
     <row r="56" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C56" s="83"/>
-      <c r="D56" s="79">
+      <c r="C56" s="85"/>
+      <c r="D56" s="88">
         <v>6</v>
       </c>
-      <c r="E56" s="79"/>
+      <c r="E56" s="88"/>
       <c r="F56">
         <v>0</v>
       </c>
@@ -3286,11 +3277,11 @@
       </c>
     </row>
     <row r="57" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C57" s="83"/>
-      <c r="D57" s="79">
+      <c r="C57" s="85"/>
+      <c r="D57" s="88">
         <v>6.5</v>
       </c>
-      <c r="E57" s="79"/>
+      <c r="E57" s="88"/>
       <c r="F57">
         <v>0</v>
       </c>
@@ -3335,11 +3326,11 @@
       </c>
     </row>
     <row r="58" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C58" s="83"/>
-      <c r="D58" s="79">
+      <c r="C58" s="85"/>
+      <c r="D58" s="88">
         <v>7</v>
       </c>
-      <c r="E58" s="79"/>
+      <c r="E58" s="88"/>
       <c r="F58">
         <v>0</v>
       </c>
@@ -3384,11 +3375,11 @@
       </c>
     </row>
     <row r="59" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C59" s="83"/>
-      <c r="D59" s="79">
+      <c r="C59" s="85"/>
+      <c r="D59" s="88">
         <v>7.5</v>
       </c>
-      <c r="E59" s="79"/>
+      <c r="E59" s="88"/>
       <c r="F59">
         <v>0</v>
       </c>
@@ -3433,11 +3424,11 @@
       </c>
     </row>
     <row r="60" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C60" s="83"/>
-      <c r="D60" s="79">
+      <c r="C60" s="85"/>
+      <c r="D60" s="88">
         <v>8</v>
       </c>
-      <c r="E60" s="79"/>
+      <c r="E60" s="88"/>
       <c r="F60">
         <v>0</v>
       </c>
@@ -3482,11 +3473,11 @@
       </c>
     </row>
     <row r="61" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C61" s="83"/>
-      <c r="D61" s="79">
+      <c r="C61" s="85"/>
+      <c r="D61" s="88">
         <v>8.5</v>
       </c>
-      <c r="E61" s="79"/>
+      <c r="E61" s="88"/>
       <c r="F61">
         <v>0</v>
       </c>
@@ -3531,11 +3522,11 @@
       </c>
     </row>
     <row r="62" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C62" s="83"/>
-      <c r="D62" s="79">
+      <c r="C62" s="85"/>
+      <c r="D62" s="88">
         <v>9</v>
       </c>
-      <c r="E62" s="79"/>
+      <c r="E62" s="88"/>
       <c r="F62">
         <v>0</v>
       </c>
@@ -3648,10 +3639,10 @@
         <v>73</v>
       </c>
       <c r="E67" s="59"/>
-      <c r="F67" s="68" t="s">
+      <c r="F67" s="93" t="s">
         <v>95</v>
       </c>
-      <c r="G67" s="69"/>
+      <c r="G67" s="94"/>
     </row>
     <row r="68" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C68" s="5" t="s">
@@ -3774,11 +3765,11 @@
     </row>
     <row r="79" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="80" spans="3:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C80" s="70" t="s">
+      <c r="C80" s="95" t="s">
         <v>82</v>
       </c>
-      <c r="D80" s="71"/>
-      <c r="E80" s="72"/>
+      <c r="D80" s="96"/>
+      <c r="E80" s="97"/>
     </row>
     <row r="81" spans="3:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C81" s="9" t="s">
@@ -3811,322 +3802,338 @@
     </row>
     <row r="87" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="88" spans="3:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C88" s="70" t="s">
-        <v>99</v>
-      </c>
-      <c r="D88" s="71"/>
-      <c r="E88" s="72"/>
+      <c r="C88" s="95"/>
+      <c r="D88" s="96"/>
+      <c r="E88" s="97"/>
     </row>
     <row r="89" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C89" s="2"/>
-      <c r="D89" s="3" t="s">
-        <v>97</v>
-      </c>
+      <c r="D89" s="3"/>
       <c r="E89" s="4"/>
-      <c r="G89" t="s">
-        <v>100</v>
-      </c>
     </row>
     <row r="90" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C90" s="9"/>
-      <c r="D90" s="58" t="s">
-        <v>98</v>
-      </c>
+      <c r="D90" s="58"/>
       <c r="E90" s="11"/>
     </row>
-    <row r="95" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="94" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="95" spans="3:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C95" s="95" t="s">
+        <v>97</v>
+      </c>
+      <c r="D95" s="96"/>
+      <c r="E95" s="97"/>
+    </row>
     <row r="96" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C96" s="87" t="s">
+      <c r="C96" s="69" t="s">
+        <v>99</v>
+      </c>
+      <c r="D96" s="70"/>
+      <c r="E96" s="70"/>
+      <c r="F96" s="70"/>
+      <c r="G96" s="70"/>
+      <c r="H96" s="71"/>
+      <c r="I96" s="72"/>
+      <c r="J96" s="68"/>
+    </row>
+    <row r="97" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C97" s="73" t="s">
+        <v>100</v>
+      </c>
+      <c r="D97" s="74"/>
+      <c r="E97" s="74"/>
+      <c r="F97" s="74"/>
+      <c r="G97" s="74"/>
+      <c r="H97" s="74"/>
+      <c r="I97" s="75"/>
+      <c r="J97" s="68"/>
+    </row>
+    <row r="98" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C98" s="76" t="s">
+        <v>101</v>
+      </c>
+      <c r="D98" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="D96" s="88"/>
-      <c r="E96" s="88"/>
-      <c r="F96" s="88"/>
-      <c r="G96" s="88"/>
-      <c r="H96" s="89"/>
-      <c r="I96" s="90"/>
-      <c r="J96" s="86"/>
-    </row>
-    <row r="97" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C97" s="91" t="s">
+      <c r="E98" s="68" t="s">
         <v>103</v>
       </c>
-      <c r="D97" s="92"/>
-      <c r="E97" s="92"/>
-      <c r="F97" s="92"/>
-      <c r="G97" s="92"/>
-      <c r="H97" s="92"/>
-      <c r="I97" s="93"/>
-      <c r="J97" s="86"/>
-    </row>
-    <row r="98" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C98" s="94" t="s">
+      <c r="F98" s="68" t="s">
         <v>104</v>
       </c>
-      <c r="D98" s="95" t="s">
+      <c r="G98" s="68" t="s">
+        <v>17</v>
+      </c>
+      <c r="H98" s="68" t="s">
         <v>105</v>
       </c>
-      <c r="E98" s="95" t="s">
+      <c r="I98" s="77" t="s">
         <v>106</v>
       </c>
-      <c r="F98" s="95" t="s">
+      <c r="J98" s="68"/>
+    </row>
+    <row r="99" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C99" s="76">
+        <v>1</v>
+      </c>
+      <c r="D99" s="68">
+        <v>80.066000000000003</v>
+      </c>
+      <c r="E99" s="68">
+        <v>2</v>
+      </c>
+      <c r="F99" s="68">
+        <v>5</v>
+      </c>
+      <c r="G99" s="68">
+        <v>0.4</v>
+      </c>
+      <c r="H99" s="68">
+        <v>0.104</v>
+      </c>
+      <c r="I99" s="77">
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="J99" s="68"/>
+    </row>
+    <row r="100" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C100" s="76">
+        <v>2</v>
+      </c>
+      <c r="D100" s="68">
+        <v>80.066000000000003</v>
+      </c>
+      <c r="E100" s="68">
+        <v>2</v>
+      </c>
+      <c r="F100" s="68">
+        <v>5</v>
+      </c>
+      <c r="G100" s="68">
+        <v>0.4</v>
+      </c>
+      <c r="H100" s="68">
+        <v>0.104</v>
+      </c>
+      <c r="I100" s="77">
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="J100" s="68"/>
+    </row>
+    <row r="101" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C101" s="76">
+        <v>3</v>
+      </c>
+      <c r="D101" s="68">
+        <v>80.066000000000003</v>
+      </c>
+      <c r="E101" s="68">
+        <v>2</v>
+      </c>
+      <c r="F101" s="68">
+        <v>5</v>
+      </c>
+      <c r="G101" s="68">
+        <v>0.2</v>
+      </c>
+      <c r="H101" s="68">
+        <v>0.104</v>
+      </c>
+      <c r="I101" s="77">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="J101" s="68" t="s">
         <v>107</v>
       </c>
-      <c r="G98" s="95" t="s">
-        <v>17</v>
-      </c>
-      <c r="H98" s="95" t="s">
+    </row>
+    <row r="102" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C102" s="76">
+        <v>4</v>
+      </c>
+      <c r="D102" s="68">
+        <v>80.066000000000003</v>
+      </c>
+      <c r="E102" s="68">
+        <v>2</v>
+      </c>
+      <c r="F102" s="68">
+        <v>8</v>
+      </c>
+      <c r="G102" s="68">
+        <v>0.25</v>
+      </c>
+      <c r="H102" s="68">
+        <v>0.104</v>
+      </c>
+      <c r="I102" s="77">
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="J102" s="68"/>
+    </row>
+    <row r="103" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C103" s="76">
+        <v>5</v>
+      </c>
+      <c r="D103" s="68">
+        <v>80.066000000000003</v>
+      </c>
+      <c r="E103" s="68">
+        <v>2</v>
+      </c>
+      <c r="F103" s="68">
+        <v>11</v>
+      </c>
+      <c r="G103" s="68">
+        <v>0.18181818199999999</v>
+      </c>
+      <c r="H103" s="68">
+        <v>0.104</v>
+      </c>
+      <c r="I103" s="77">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="J103" s="68"/>
+    </row>
+    <row r="104" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C104" s="78">
+        <v>6</v>
+      </c>
+      <c r="D104" s="74">
+        <v>80.066000000000003</v>
+      </c>
+      <c r="E104" s="74">
+        <v>2</v>
+      </c>
+      <c r="F104" s="74" t="s">
+        <v>111</v>
+      </c>
+      <c r="G104" s="74" t="s">
+        <v>110</v>
+      </c>
+      <c r="H104" s="74">
+        <v>0.104</v>
+      </c>
+      <c r="I104" s="79" t="s">
         <v>108</v>
       </c>
-      <c r="I98" s="96" t="s">
+      <c r="J104" s="68"/>
+    </row>
+    <row r="105" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C105" s="78">
+        <v>7</v>
+      </c>
+      <c r="D105" s="74">
+        <v>80.066000000000003</v>
+      </c>
+      <c r="E105" s="74">
+        <v>2</v>
+      </c>
+      <c r="F105" s="74" t="s">
+        <v>111</v>
+      </c>
+      <c r="G105" s="74" t="s">
+        <v>110</v>
+      </c>
+      <c r="H105" s="74">
+        <v>0.104</v>
+      </c>
+      <c r="I105" s="79" t="s">
+        <v>108</v>
+      </c>
+      <c r="J105" s="68"/>
+    </row>
+    <row r="106" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C106" s="78">
+        <v>8</v>
+      </c>
+      <c r="D106" s="74">
+        <v>80.066000000000003</v>
+      </c>
+      <c r="E106" s="74">
+        <v>2</v>
+      </c>
+      <c r="F106" s="74" t="s">
+        <v>111</v>
+      </c>
+      <c r="G106" s="74" t="s">
+        <v>110</v>
+      </c>
+      <c r="H106" s="74">
+        <v>0.104</v>
+      </c>
+      <c r="I106" s="79" t="s">
+        <v>108</v>
+      </c>
+      <c r="J106" s="68"/>
+    </row>
+    <row r="107" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C107" s="78">
+        <v>9</v>
+      </c>
+      <c r="D107" s="74">
+        <v>80.066000000000003</v>
+      </c>
+      <c r="E107" s="74">
+        <v>2</v>
+      </c>
+      <c r="F107" s="74" t="s">
+        <v>111</v>
+      </c>
+      <c r="G107" s="74" t="s">
+        <v>110</v>
+      </c>
+      <c r="H107" s="74">
+        <v>0.104</v>
+      </c>
+      <c r="I107" s="79" t="s">
+        <v>108</v>
+      </c>
+      <c r="J107" s="68"/>
+    </row>
+    <row r="108" spans="3:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C108" s="80">
+        <v>10</v>
+      </c>
+      <c r="D108" s="81">
+        <v>80.066000000000003</v>
+      </c>
+      <c r="E108" s="81">
+        <v>2</v>
+      </c>
+      <c r="F108" s="81">
+        <v>8.6</v>
+      </c>
+      <c r="G108" s="81"/>
+      <c r="H108" s="81">
+        <v>0.104</v>
+      </c>
+      <c r="I108" s="82">
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="J108" s="68" t="s">
         <v>109</v>
       </c>
-      <c r="J98" s="86"/>
-    </row>
-    <row r="99" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C99" s="94">
-        <v>1</v>
-      </c>
-      <c r="D99" s="95">
-        <v>80.066000000000003</v>
-      </c>
-      <c r="E99" s="95">
-        <v>2</v>
-      </c>
-      <c r="F99" s="95">
-        <v>5</v>
-      </c>
-      <c r="G99" s="95">
-        <v>0.4</v>
-      </c>
-      <c r="H99" s="95">
-        <v>0.104</v>
-      </c>
-      <c r="I99" s="96">
-        <v>0.26100000000000001</v>
-      </c>
-      <c r="J99" s="86"/>
-    </row>
-    <row r="100" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C100" s="94">
-        <v>2</v>
-      </c>
-      <c r="D100" s="95">
-        <v>80.066000000000003</v>
-      </c>
-      <c r="E100" s="95">
-        <v>2</v>
-      </c>
-      <c r="F100" s="95">
-        <v>5</v>
-      </c>
-      <c r="G100" s="95">
-        <v>0.4</v>
-      </c>
-      <c r="H100" s="95">
-        <v>0.104</v>
-      </c>
-      <c r="I100" s="96">
-        <v>0.26100000000000001</v>
-      </c>
-      <c r="J100" s="86"/>
-    </row>
-    <row r="101" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C101" s="94">
-        <v>3</v>
-      </c>
-      <c r="D101" s="95">
-        <v>80.066000000000003</v>
-      </c>
-      <c r="E101" s="95">
-        <v>2</v>
-      </c>
-      <c r="F101" s="95">
-        <v>5</v>
-      </c>
-      <c r="G101" s="95">
-        <v>0.2</v>
-      </c>
-      <c r="H101" s="95">
-        <v>0.104</v>
-      </c>
-      <c r="I101" s="96">
-        <v>0.52200000000000002</v>
-      </c>
-      <c r="J101" s="86" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="102" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C102" s="94">
-        <v>4</v>
-      </c>
-      <c r="D102" s="95">
-        <v>80.066000000000003</v>
-      </c>
-      <c r="E102" s="95">
-        <v>2</v>
-      </c>
-      <c r="F102" s="95">
-        <v>8</v>
-      </c>
-      <c r="G102" s="95">
-        <v>0.25</v>
-      </c>
-      <c r="H102" s="95">
-        <v>0.104</v>
-      </c>
-      <c r="I102" s="96">
-        <v>0.41699999999999998</v>
-      </c>
-      <c r="J102" s="86"/>
-    </row>
-    <row r="103" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C103" s="94">
-        <v>5</v>
-      </c>
-      <c r="D103" s="95">
-        <v>80.066000000000003</v>
-      </c>
-      <c r="E103" s="95">
-        <v>2</v>
-      </c>
-      <c r="F103" s="95">
-        <v>11</v>
-      </c>
-      <c r="G103" s="95">
-        <v>0.18181818199999999</v>
-      </c>
-      <c r="H103" s="95">
-        <v>0.104</v>
-      </c>
-      <c r="I103" s="96">
-        <v>0.57899999999999996</v>
-      </c>
-      <c r="J103" s="86"/>
-    </row>
-    <row r="104" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C104" s="97">
-        <v>6</v>
-      </c>
-      <c r="D104" s="92">
-        <v>80.066000000000003</v>
-      </c>
-      <c r="E104" s="92">
-        <v>2</v>
-      </c>
-      <c r="F104" s="92" t="s">
-        <v>114</v>
-      </c>
-      <c r="G104" s="92" t="s">
-        <v>113</v>
-      </c>
-      <c r="H104" s="92">
-        <v>0.104</v>
-      </c>
-      <c r="I104" s="98" t="s">
-        <v>111</v>
-      </c>
-      <c r="J104" s="86"/>
-    </row>
-    <row r="105" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C105" s="97">
-        <v>7</v>
-      </c>
-      <c r="D105" s="92">
-        <v>80.066000000000003</v>
-      </c>
-      <c r="E105" s="92">
-        <v>2</v>
-      </c>
-      <c r="F105" s="92" t="s">
-        <v>114</v>
-      </c>
-      <c r="G105" s="92" t="s">
-        <v>113</v>
-      </c>
-      <c r="H105" s="92">
-        <v>0.104</v>
-      </c>
-      <c r="I105" s="98" t="s">
-        <v>111</v>
-      </c>
-      <c r="J105" s="86"/>
-    </row>
-    <row r="106" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C106" s="97">
-        <v>8</v>
-      </c>
-      <c r="D106" s="92">
-        <v>80.066000000000003</v>
-      </c>
-      <c r="E106" s="92">
-        <v>2</v>
-      </c>
-      <c r="F106" s="92" t="s">
-        <v>114</v>
-      </c>
-      <c r="G106" s="92" t="s">
-        <v>113</v>
-      </c>
-      <c r="H106" s="92">
-        <v>0.104</v>
-      </c>
-      <c r="I106" s="98" t="s">
-        <v>111</v>
-      </c>
-      <c r="J106" s="86"/>
-    </row>
-    <row r="107" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C107" s="97">
-        <v>9</v>
-      </c>
-      <c r="D107" s="92">
-        <v>80.066000000000003</v>
-      </c>
-      <c r="E107" s="92">
-        <v>2</v>
-      </c>
-      <c r="F107" s="92" t="s">
-        <v>114</v>
-      </c>
-      <c r="G107" s="92" t="s">
-        <v>113</v>
-      </c>
-      <c r="H107" s="92">
-        <v>0.104</v>
-      </c>
-      <c r="I107" s="98" t="s">
-        <v>111</v>
-      </c>
-      <c r="J107" s="86"/>
-    </row>
-    <row r="108" spans="3:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C108" s="99">
-        <v>10</v>
-      </c>
-      <c r="D108" s="100">
-        <v>80.066000000000003</v>
-      </c>
-      <c r="E108" s="100">
-        <v>2</v>
-      </c>
-      <c r="F108" s="100">
-        <v>8.6</v>
-      </c>
-      <c r="G108" s="100"/>
-      <c r="H108" s="100">
-        <v>0.104</v>
-      </c>
-      <c r="I108" s="101">
-        <v>0.45300000000000001</v>
-      </c>
-      <c r="J108" s="86" t="s">
-        <v>112</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="31">
+  <mergeCells count="32">
+    <mergeCell ref="C95:E95"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="C88:E88"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="C80:E80"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="G30:I30"/>
     <mergeCell ref="J37:Y37"/>
     <mergeCell ref="J49:S49"/>
     <mergeCell ref="C39:C43"/>
@@ -4141,23 +4148,6 @@
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="D59:E59"/>
     <mergeCell ref="D60:E60"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="C88:E88"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="C80:E80"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="F49:I49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix spreadsheet transmission factors 0.513 -> 0.13
</commit_message>
<xml_diff>
--- a/Studies/USMap_Doubleday_2024/SETUPS Description Complete_sil.xlsx
+++ b/Studies/USMap_Doubleday_2024/SETUPS Description Complete_sil.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tford\dev\InSPIRE\Studies\USMap_Doubleday_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1A2BFF-A824-4EBB-BF2E-3EFAB88E3E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD32F2A-FF4E-44BF-BFD7-EC398CB41F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-4470" windowWidth="16440" windowHeight="28320" xr2:uid="{20F8F7F2-6405-4778-91BF-D0B7AC5935BA}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -874,7 +873,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -898,7 +897,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1024,6 +1022,45 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1037,45 +1074,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1500,8 +1498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932A1107-9899-4DFE-A9E6-0ED2844D3F4A}">
   <dimension ref="B2:AA108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J92" sqref="J92"/>
+    <sheetView tabSelected="1" topLeftCell="D3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1522,71 +1520,71 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="T2" s="89" t="s">
+      <c r="T2" s="91" t="s">
         <v>60</v>
       </c>
-      <c r="U2" s="89"/>
+      <c r="U2" s="91"/>
     </row>
     <row r="3" spans="2:21" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="25" t="s">
+      <c r="B3" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="25" t="s">
+      <c r="I3" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="25" t="s">
+      <c r="J3" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="25" t="s">
+      <c r="K3" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25" t="s">
+      <c r="L3" s="24"/>
+      <c r="M3" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="25" t="s">
+      <c r="N3" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="O3" s="25" t="s">
+      <c r="O3" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="P3" s="25" t="s">
+      <c r="P3" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="25" t="s">
+      <c r="Q3" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="R3" s="26" t="s">
+      <c r="R3" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="S3" s="67" t="s">
+      <c r="S3" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="T3" s="25" t="s">
+      <c r="T3" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="U3" s="25" t="s">
+      <c r="U3" s="24" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1624,7 +1622,7 @@
       <c r="L4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="27" t="s">
+      <c r="M4" s="26" t="s">
         <v>14</v>
       </c>
       <c r="N4">
@@ -1642,7 +1640,7 @@
       <c r="R4" s="4">
         <v>20</v>
       </c>
-      <c r="T4" s="27"/>
+      <c r="T4" s="26"/>
       <c r="U4" s="3"/>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.25">
@@ -1676,7 +1674,7 @@
       <c r="K5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M5" s="28" t="s">
+      <c r="M5" s="27" t="s">
         <v>14</v>
       </c>
       <c r="N5">
@@ -1694,7 +1692,7 @@
       <c r="R5" s="6">
         <v>20</v>
       </c>
-      <c r="T5" s="28"/>
+      <c r="T5" s="27"/>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B6" s="5">
@@ -1715,8 +1713,8 @@
       <c r="G6">
         <v>1</v>
       </c>
-      <c r="H6" s="19">
-        <v>0.51300000000000001</v>
+      <c r="H6">
+        <v>0.13</v>
       </c>
       <c r="I6" t="s">
         <v>10</v>
@@ -1727,7 +1725,7 @@
       <c r="K6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M6" s="28" t="s">
+      <c r="M6" s="27" t="s">
         <v>14</v>
       </c>
       <c r="N6">
@@ -1745,7 +1743,7 @@
       <c r="R6" s="6">
         <v>20</v>
       </c>
-      <c r="T6" s="28"/>
+      <c r="T6" s="27"/>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B7" s="5">
@@ -1778,7 +1776,7 @@
       <c r="K7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="28" t="s">
+      <c r="M7" s="27" t="s">
         <v>14</v>
       </c>
       <c r="N7">
@@ -1796,7 +1794,7 @@
       <c r="R7" s="6">
         <v>20</v>
       </c>
-      <c r="T7" s="28"/>
+      <c r="T7" s="27"/>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B8" s="5">
@@ -1829,7 +1827,7 @@
       <c r="K8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M8" s="28" t="s">
+      <c r="M8" s="27" t="s">
         <v>14</v>
       </c>
       <c r="N8">
@@ -1847,10 +1845,10 @@
       <c r="R8" s="6">
         <v>20</v>
       </c>
-      <c r="T8" s="28"/>
+      <c r="T8" s="27"/>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B9" s="65" t="s">
+      <c r="B9" s="64" t="s">
         <v>96</v>
       </c>
       <c r="C9">
@@ -1859,9 +1857,9 @@
       <c r="E9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-      <c r="M9" s="28"/>
+      <c r="M9" s="27"/>
       <c r="R9" s="6"/>
-      <c r="T9" s="28"/>
+      <c r="T9" s="27"/>
     </row>
     <row r="10" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
@@ -1873,7 +1871,7 @@
       <c r="D10">
         <v>1.5</v>
       </c>
-      <c r="E10" s="32" t="s">
+      <c r="E10" s="31" t="s">
         <v>61</v>
       </c>
       <c r="F10">
@@ -1894,13 +1892,13 @@
       <c r="K10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M10" s="29" t="s">
+      <c r="M10" s="28" t="s">
         <v>21</v>
       </c>
       <c r="N10">
         <v>0.3</v>
       </c>
-      <c r="O10" s="21" t="s">
+      <c r="O10" s="20" t="s">
         <v>14</v>
       </c>
       <c r="P10">
@@ -1915,8 +1913,8 @@
       <c r="S10" t="s">
         <v>98</v>
       </c>
-      <c r="T10" s="28"/>
-      <c r="U10" s="20"/>
+      <c r="T10" s="27"/>
+      <c r="U10" s="19"/>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B11" s="5">
@@ -1928,7 +1926,7 @@
       <c r="D11">
         <v>2.4</v>
       </c>
-      <c r="E11" s="32" t="s">
+      <c r="E11" s="31" t="s">
         <v>61</v>
       </c>
       <c r="F11">
@@ -1949,13 +1947,13 @@
       <c r="K11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M11" s="29" t="s">
+      <c r="M11" s="28" t="s">
         <v>21</v>
       </c>
       <c r="N11">
         <v>0.3</v>
       </c>
-      <c r="O11" s="21" t="s">
+      <c r="O11" s="20" t="s">
         <v>14</v>
       </c>
       <c r="P11">
@@ -1970,8 +1968,8 @@
       <c r="S11" t="s">
         <v>98</v>
       </c>
-      <c r="T11" s="28"/>
-      <c r="U11" s="20"/>
+      <c r="T11" s="27"/>
+      <c r="U11" s="19"/>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B12" s="5">
@@ -1983,7 +1981,7 @@
       <c r="D12">
         <v>2.4</v>
       </c>
-      <c r="E12" s="32" t="s">
+      <c r="E12" s="31" t="s">
         <v>61</v>
       </c>
       <c r="F12">
@@ -1992,8 +1990,8 @@
       <c r="G12">
         <v>1</v>
       </c>
-      <c r="H12" s="19">
-        <v>0.51300000000000001</v>
+      <c r="H12">
+        <v>0.13</v>
       </c>
       <c r="I12" t="s">
         <v>10</v>
@@ -2004,7 +2002,7 @@
       <c r="K12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M12" s="29" t="s">
+      <c r="M12" s="28" t="s">
         <v>21</v>
       </c>
       <c r="N12">
@@ -2025,8 +2023,8 @@
       <c r="S12" t="s">
         <v>98</v>
       </c>
-      <c r="T12" s="28"/>
-      <c r="U12" s="20"/>
+      <c r="T12" s="27"/>
+      <c r="U12" s="19"/>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B13" s="5">
@@ -2038,7 +2036,7 @@
       <c r="D13">
         <v>1.5</v>
       </c>
-      <c r="E13" s="32" t="s">
+      <c r="E13" s="31" t="s">
         <v>61</v>
       </c>
       <c r="F13">
@@ -2059,7 +2057,7 @@
       <c r="K13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M13" s="29" t="s">
+      <c r="M13" s="28" t="s">
         <v>21</v>
       </c>
       <c r="N13">
@@ -2080,8 +2078,8 @@
       <c r="S13" t="s">
         <v>98</v>
       </c>
-      <c r="T13" s="28"/>
-      <c r="U13" s="20"/>
+      <c r="T13" s="27"/>
+      <c r="U13" s="19"/>
     </row>
     <row r="14" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="9">
@@ -2090,10 +2088,10 @@
       <c r="C14" s="10">
         <v>0.6</v>
       </c>
-      <c r="D14" s="22">
+      <c r="D14" s="21">
         <v>2</v>
       </c>
-      <c r="E14" s="23">
+      <c r="E14" s="22">
         <v>8.6</v>
       </c>
       <c r="F14" s="10">
@@ -2108,20 +2106,20 @@
       <c r="I14" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="J14" s="23" t="s">
+      <c r="J14" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="K14" s="23" t="s">
+      <c r="K14" s="22" t="s">
         <v>15</v>
       </c>
       <c r="L14" s="10"/>
-      <c r="M14" s="30">
+      <c r="M14" s="29">
         <v>90</v>
       </c>
-      <c r="N14" s="30">
+      <c r="N14" s="29">
         <v>0.23255813953488372</v>
       </c>
-      <c r="O14" s="23" t="s">
+      <c r="O14" s="22" t="s">
         <v>14</v>
       </c>
       <c r="P14" s="10">
@@ -2133,7 +2131,7 @@
       <c r="R14" s="11">
         <v>20</v>
       </c>
-      <c r="T14" s="30">
+      <c r="T14" s="29">
         <f>2/E14</f>
         <v>0.23255813953488372</v>
       </c>
@@ -2196,25 +2194,25 @@
       <c r="D19">
         <v>25</v>
       </c>
-      <c r="E19" s="33">
+      <c r="E19" s="32">
         <f>2*COS(RADIANS(D19))</f>
         <v>1.8126155740732999</v>
       </c>
       <c r="F19">
         <v>2</v>
       </c>
-      <c r="G19" s="33">
+      <c r="G19" s="32">
         <f>F19+E19</f>
         <v>3.8126155740733001</v>
       </c>
-      <c r="H19" s="34">
+      <c r="H19" s="33">
         <f>B19/G19</f>
         <v>0.52457426172218347</v>
       </c>
-      <c r="I19" s="34">
+      <c r="I19" s="33">
         <v>0.65</v>
       </c>
-      <c r="J19" s="34">
+      <c r="J19" s="33">
         <f>2/I19</f>
         <v>3.0769230769230766</v>
       </c>
@@ -2230,22 +2228,22 @@
       <c r="D20">
         <v>40</v>
       </c>
-      <c r="E20" s="33">
+      <c r="E20" s="32">
         <f>2*COS(RADIANS(D20))</f>
         <v>1.532088886237956</v>
       </c>
       <c r="F20">
         <v>2</v>
       </c>
-      <c r="G20" s="33">
+      <c r="G20" s="32">
         <f>F20+E20</f>
         <v>3.5320888862379558</v>
       </c>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34">
+      <c r="H20" s="33"/>
+      <c r="I20" s="33">
         <v>0.25</v>
       </c>
-      <c r="J20" s="34">
+      <c r="J20" s="33">
         <f>2/I20</f>
         <v>8</v>
       </c>
@@ -2253,7 +2251,7 @@
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
-      <c r="H21" s="34"/>
+      <c r="H21" s="33"/>
       <c r="K21" s="6"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
@@ -2270,7 +2268,7 @@
       <c r="G22">
         <v>0.18</v>
       </c>
-      <c r="H22" s="34">
+      <c r="H22" s="33">
         <f>F22/G22</f>
         <v>11.111111111111111</v>
       </c>
@@ -2290,7 +2288,7 @@
       <c r="G23">
         <v>0.4</v>
       </c>
-      <c r="H23" s="34">
+      <c r="H23" s="33">
         <f t="shared" ref="H23:H25" si="0">F23/G23</f>
         <v>5</v>
       </c>
@@ -2304,7 +2302,7 @@
       <c r="G24">
         <v>0.6</v>
       </c>
-      <c r="H24" s="34">
+      <c r="H24" s="33">
         <f t="shared" si="0"/>
         <v>3.3333333333333335</v>
       </c>
@@ -2321,7 +2319,7 @@
       <c r="G25" s="10">
         <v>0.8</v>
       </c>
-      <c r="H25" s="35">
+      <c r="H25" s="34">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
@@ -2338,11 +2336,11 @@
       <c r="D27" s="13"/>
       <c r="E27" s="13"/>
       <c r="F27" s="14"/>
-      <c r="G27" s="90" t="s">
+      <c r="G27" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="H27" s="91"/>
-      <c r="I27" s="91"/>
+      <c r="H27" s="93"/>
+      <c r="I27" s="93"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
@@ -2352,9 +2350,9 @@
         <v>8</v>
       </c>
       <c r="F28" s="6"/>
-      <c r="G28" s="92"/>
-      <c r="H28" s="88"/>
-      <c r="I28" s="88"/>
+      <c r="G28" s="94"/>
+      <c r="H28" s="89"/>
+      <c r="I28" s="89"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
@@ -2364,9 +2362,9 @@
         <v>2</v>
       </c>
       <c r="F29" s="6"/>
-      <c r="G29" s="92"/>
-      <c r="H29" s="88"/>
-      <c r="I29" s="88"/>
+      <c r="G29" s="94"/>
+      <c r="H29" s="89"/>
+      <c r="I29" s="89"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
@@ -2384,9 +2382,9 @@
       <c r="F30" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G30" s="92"/>
-      <c r="H30" s="88"/>
-      <c r="I30" s="88"/>
+      <c r="G30" s="94"/>
+      <c r="H30" s="89"/>
+      <c r="I30" s="89"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
@@ -2408,11 +2406,11 @@
         <f>ROUND(D31/10,0)</f>
         <v>3</v>
       </c>
-      <c r="G31" s="98" t="s">
+      <c r="G31" s="87" t="s">
         <v>37</v>
       </c>
-      <c r="H31" s="99"/>
-      <c r="I31" s="99"/>
+      <c r="H31" s="88"/>
+      <c r="I31" s="88"/>
     </row>
     <row r="32" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="9" t="s">
@@ -2434,118 +2432,118 @@
         <f>ROUND(D32/10,0)</f>
         <v>8</v>
       </c>
-      <c r="G32" s="98" t="s">
+      <c r="G32" s="87" t="s">
         <v>38</v>
       </c>
-      <c r="H32" s="99"/>
-      <c r="I32" s="99"/>
+      <c r="H32" s="88"/>
+      <c r="I32" s="88"/>
     </row>
     <row r="36" spans="3:26" x14ac:dyDescent="0.25">
       <c r="O36"/>
     </row>
     <row r="37" spans="3:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="83"/>
-      <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="100" t="s">
+      <c r="C37" s="95"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="90" t="s">
         <v>59</v>
       </c>
-      <c r="G37" s="100"/>
-      <c r="H37" s="100"/>
-      <c r="I37" s="100"/>
-      <c r="J37" s="83" t="s">
+      <c r="G37" s="90"/>
+      <c r="H37" s="90"/>
+      <c r="I37" s="90"/>
+      <c r="J37" s="95" t="s">
         <v>58</v>
       </c>
-      <c r="K37" s="83"/>
-      <c r="L37" s="83"/>
-      <c r="M37" s="83"/>
-      <c r="N37" s="83"/>
-      <c r="O37" s="83"/>
-      <c r="P37" s="83"/>
-      <c r="Q37" s="83"/>
-      <c r="R37" s="83"/>
-      <c r="S37" s="83"/>
-      <c r="T37" s="83"/>
-      <c r="U37" s="83"/>
-      <c r="V37" s="83"/>
-      <c r="W37" s="83"/>
-      <c r="X37" s="83"/>
-      <c r="Y37" s="83"/>
-    </row>
-    <row r="38" spans="3:26" s="37" customFormat="1" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C38" s="83"/>
-      <c r="D38" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="E38" s="38" t="s">
+      <c r="K37" s="95"/>
+      <c r="L37" s="95"/>
+      <c r="M37" s="95"/>
+      <c r="N37" s="95"/>
+      <c r="O37" s="95"/>
+      <c r="P37" s="95"/>
+      <c r="Q37" s="95"/>
+      <c r="R37" s="95"/>
+      <c r="S37" s="95"/>
+      <c r="T37" s="95"/>
+      <c r="U37" s="95"/>
+      <c r="V37" s="95"/>
+      <c r="W37" s="95"/>
+      <c r="X37" s="95"/>
+      <c r="Y37" s="95"/>
+    </row>
+    <row r="38" spans="3:26" s="36" customFormat="1" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C38" s="95"/>
+      <c r="D38" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="E38" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="F38" s="39" t="s">
+      <c r="F38" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="G38" s="39" t="s">
+      <c r="G38" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="H38" s="39" t="s">
+      <c r="H38" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="I38" s="39" t="s">
+      <c r="I38" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="J38" s="40" t="s">
+      <c r="J38" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="K38" s="40" t="s">
+      <c r="K38" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="L38" s="40" t="s">
+      <c r="L38" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="M38" s="40" t="s">
+      <c r="M38" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="N38" s="42" t="s">
+      <c r="N38" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="O38" s="43" t="s">
+      <c r="O38" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="P38" s="44" t="s">
+      <c r="P38" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="Q38" s="44" t="s">
+      <c r="Q38" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="R38" s="41" t="s">
+      <c r="R38" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="S38" s="45" t="s">
+      <c r="S38" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="T38" s="46" t="s">
+      <c r="T38" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="U38" s="47" t="s">
+      <c r="U38" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="V38" s="48" t="s">
+      <c r="V38" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="W38" s="48" t="s">
+      <c r="W38" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="X38" s="49" t="s">
+      <c r="X38" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="Y38" s="50" t="s">
+      <c r="Y38" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="Z38" s="62" t="s">
+      <c r="Z38" s="61" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="39" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C39" s="84" t="s">
+      <c r="C39" s="96" t="s">
         <v>66</v>
       </c>
       <c r="D39">
@@ -2598,7 +2596,7 @@
       </c>
     </row>
     <row r="40" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C40" s="84"/>
+      <c r="C40" s="96"/>
       <c r="D40">
         <v>2</v>
       </c>
@@ -2649,7 +2647,7 @@
       </c>
     </row>
     <row r="41" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C41" s="84"/>
+      <c r="C41" s="96"/>
       <c r="D41">
         <v>3</v>
       </c>
@@ -2700,7 +2698,7 @@
       </c>
     </row>
     <row r="42" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C42" s="84"/>
+      <c r="C42" s="96"/>
       <c r="D42">
         <v>4</v>
       </c>
@@ -2751,7 +2749,7 @@
       </c>
     </row>
     <row r="43" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C43" s="84"/>
+      <c r="C43" s="96"/>
       <c r="D43">
         <v>5</v>
       </c>
@@ -2820,7 +2818,7 @@
       </c>
     </row>
     <row r="44" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C44" s="51" t="s">
+      <c r="C44" s="50" t="s">
         <v>67</v>
       </c>
       <c r="D44">
@@ -2907,87 +2905,87 @@
       <c r="O48"/>
     </row>
     <row r="49" spans="3:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C49" s="85" t="s">
+      <c r="C49" s="97" t="s">
         <v>68</v>
       </c>
-      <c r="D49" s="87" t="s">
+      <c r="D49" s="99" t="s">
         <v>62</v>
       </c>
-      <c r="E49" s="87"/>
-      <c r="F49" s="100" t="s">
+      <c r="E49" s="99"/>
+      <c r="F49" s="90" t="s">
         <v>59</v>
       </c>
-      <c r="G49" s="100"/>
-      <c r="H49" s="100"/>
-      <c r="I49" s="100"/>
-      <c r="J49" s="83" t="s">
+      <c r="G49" s="90"/>
+      <c r="H49" s="90"/>
+      <c r="I49" s="90"/>
+      <c r="J49" s="95" t="s">
         <v>58</v>
       </c>
-      <c r="K49" s="83"/>
-      <c r="L49" s="83"/>
-      <c r="M49" s="83"/>
-      <c r="N49" s="83"/>
-      <c r="O49" s="83"/>
-      <c r="P49" s="83"/>
-      <c r="Q49" s="83"/>
-      <c r="R49" s="83"/>
-      <c r="S49" s="83"/>
+      <c r="K49" s="95"/>
+      <c r="L49" s="95"/>
+      <c r="M49" s="95"/>
+      <c r="N49" s="95"/>
+      <c r="O49" s="95"/>
+      <c r="P49" s="95"/>
+      <c r="Q49" s="95"/>
+      <c r="R49" s="95"/>
+      <c r="S49" s="95"/>
     </row>
     <row r="50" spans="3:19" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C50" s="85"/>
-      <c r="D50" s="86" t="s">
+      <c r="C50" s="97"/>
+      <c r="D50" s="98" t="s">
         <v>63</v>
       </c>
-      <c r="E50" s="86"/>
-      <c r="F50" s="39" t="s">
+      <c r="E50" s="98"/>
+      <c r="F50" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="G50" s="39" t="s">
+      <c r="G50" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="H50" s="39" t="s">
+      <c r="H50" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="I50" s="39" t="s">
+      <c r="I50" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="J50" s="40" t="s">
+      <c r="J50" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="K50" s="40" t="s">
+      <c r="K50" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="L50" s="40" t="s">
+      <c r="L50" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="M50" s="40" t="s">
+      <c r="M50" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="N50" s="42" t="s">
+      <c r="N50" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="O50" s="43" t="s">
+      <c r="O50" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="P50" s="44" t="s">
+      <c r="P50" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="Q50" s="44" t="s">
+      <c r="Q50" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="R50" s="41" t="s">
+      <c r="R50" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="S50" s="45" t="s">
+      <c r="S50" s="44" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="51" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C51" s="85"/>
-      <c r="D51" s="88">
+      <c r="C51" s="97"/>
+      <c r="D51" s="89">
         <v>3.8</v>
       </c>
-      <c r="E51" s="88"/>
+      <c r="E51" s="89"/>
       <c r="F51">
         <v>0</v>
       </c>
@@ -3032,11 +3030,11 @@
       </c>
     </row>
     <row r="52" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C52" s="85"/>
-      <c r="D52" s="88">
+      <c r="C52" s="97"/>
+      <c r="D52" s="89">
         <v>4</v>
       </c>
-      <c r="E52" s="88"/>
+      <c r="E52" s="89"/>
       <c r="F52">
         <v>0</v>
       </c>
@@ -3081,11 +3079,11 @@
       </c>
     </row>
     <row r="53" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C53" s="85"/>
-      <c r="D53" s="88">
+      <c r="C53" s="97"/>
+      <c r="D53" s="89">
         <v>4.5</v>
       </c>
-      <c r="E53" s="88"/>
+      <c r="E53" s="89"/>
       <c r="F53">
         <v>0</v>
       </c>
@@ -3130,11 +3128,11 @@
       </c>
     </row>
     <row r="54" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C54" s="85"/>
-      <c r="D54" s="88">
+      <c r="C54" s="97"/>
+      <c r="D54" s="89">
         <v>5</v>
       </c>
-      <c r="E54" s="88"/>
+      <c r="E54" s="89"/>
       <c r="F54">
         <v>0</v>
       </c>
@@ -3179,11 +3177,11 @@
       </c>
     </row>
     <row r="55" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C55" s="85"/>
-      <c r="D55" s="88">
+      <c r="C55" s="97"/>
+      <c r="D55" s="89">
         <v>5.5</v>
       </c>
-      <c r="E55" s="88"/>
+      <c r="E55" s="89"/>
       <c r="F55">
         <v>0</v>
       </c>
@@ -3228,11 +3226,11 @@
       </c>
     </row>
     <row r="56" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C56" s="85"/>
-      <c r="D56" s="88">
+      <c r="C56" s="97"/>
+      <c r="D56" s="89">
         <v>6</v>
       </c>
-      <c r="E56" s="88"/>
+      <c r="E56" s="89"/>
       <c r="F56">
         <v>0</v>
       </c>
@@ -3277,11 +3275,11 @@
       </c>
     </row>
     <row r="57" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C57" s="85"/>
-      <c r="D57" s="88">
+      <c r="C57" s="97"/>
+      <c r="D57" s="89">
         <v>6.5</v>
       </c>
-      <c r="E57" s="88"/>
+      <c r="E57" s="89"/>
       <c r="F57">
         <v>0</v>
       </c>
@@ -3326,11 +3324,11 @@
       </c>
     </row>
     <row r="58" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C58" s="85"/>
-      <c r="D58" s="88">
+      <c r="C58" s="97"/>
+      <c r="D58" s="89">
         <v>7</v>
       </c>
-      <c r="E58" s="88"/>
+      <c r="E58" s="89"/>
       <c r="F58">
         <v>0</v>
       </c>
@@ -3375,11 +3373,11 @@
       </c>
     </row>
     <row r="59" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C59" s="85"/>
-      <c r="D59" s="88">
+      <c r="C59" s="97"/>
+      <c r="D59" s="89">
         <v>7.5</v>
       </c>
-      <c r="E59" s="88"/>
+      <c r="E59" s="89"/>
       <c r="F59">
         <v>0</v>
       </c>
@@ -3424,11 +3422,11 @@
       </c>
     </row>
     <row r="60" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C60" s="85"/>
-      <c r="D60" s="88">
+      <c r="C60" s="97"/>
+      <c r="D60" s="89">
         <v>8</v>
       </c>
-      <c r="E60" s="88"/>
+      <c r="E60" s="89"/>
       <c r="F60">
         <v>0</v>
       </c>
@@ -3473,11 +3471,11 @@
       </c>
     </row>
     <row r="61" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C61" s="85"/>
-      <c r="D61" s="88">
+      <c r="C61" s="97"/>
+      <c r="D61" s="89">
         <v>8.5</v>
       </c>
-      <c r="E61" s="88"/>
+      <c r="E61" s="89"/>
       <c r="F61">
         <v>0</v>
       </c>
@@ -3522,11 +3520,11 @@
       </c>
     </row>
     <row r="62" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C62" s="85"/>
-      <c r="D62" s="88">
+      <c r="C62" s="97"/>
+      <c r="D62" s="89">
         <v>9</v>
       </c>
-      <c r="E62" s="88"/>
+      <c r="E62" s="89"/>
       <c r="F62">
         <v>0</v>
       </c>
@@ -3626,11 +3624,11 @@
       <c r="O65"/>
     </row>
     <row r="66" spans="3:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C66" s="55" t="s">
+      <c r="C66" s="54" t="s">
         <v>69</v>
       </c>
-      <c r="D66" s="56"/>
-      <c r="E66" s="57"/>
+      <c r="D66" s="55"/>
+      <c r="E66" s="56"/>
       <c r="O66"/>
       <c r="AA66" s="1"/>
     </row>
@@ -3638,27 +3636,27 @@
       <c r="C67" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E67" s="59"/>
-      <c r="F67" s="93" t="s">
+      <c r="E67" s="58"/>
+      <c r="F67" s="85" t="s">
         <v>95</v>
       </c>
-      <c r="G67" s="94"/>
+      <c r="G67" s="86"/>
     </row>
     <row r="68" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C68" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D68" s="52">
+      <c r="D68" s="51">
         <f>F68*0.3048</f>
         <v>0.15240000000000001</v>
       </c>
-      <c r="E68" s="59" t="s">
+      <c r="E68" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="F68" s="63">
+      <c r="F68" s="62">
         <v>0.5</v>
       </c>
-      <c r="G68" s="64" t="s">
+      <c r="G68" s="63" t="s">
         <v>71</v>
       </c>
     </row>
@@ -3666,10 +3664,10 @@
       <c r="C69" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D69" s="52">
+      <c r="D69" s="51">
         <v>5</v>
       </c>
-      <c r="E69" s="59" t="s">
+      <c r="E69" s="58" t="s">
         <v>74</v>
       </c>
     </row>
@@ -3677,10 +3675,10 @@
       <c r="C70" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D70" s="52">
+      <c r="D70" s="51">
         <v>2</v>
       </c>
-      <c r="E70" s="59" t="s">
+      <c r="E70" s="58" t="s">
         <v>74</v>
       </c>
     </row>
@@ -3691,7 +3689,7 @@
       <c r="D71">
         <v>0</v>
       </c>
-      <c r="E71" s="59" t="s">
+      <c r="E71" s="58" t="s">
         <v>78</v>
       </c>
     </row>
@@ -3703,7 +3701,7 @@
         <f>D70/D69</f>
         <v>0.4</v>
       </c>
-      <c r="E72" s="59"/>
+      <c r="E72" s="58"/>
     </row>
     <row r="73" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C73" s="5" t="s">
@@ -3713,7 +3711,7 @@
         <f>D70*COS(RADIANS(D71))</f>
         <v>2</v>
       </c>
-      <c r="E73" s="61" t="s">
+      <c r="E73" s="60" t="s">
         <v>81</v>
       </c>
     </row>
@@ -3725,7 +3723,7 @@
         <f>D69-D73</f>
         <v>3</v>
       </c>
-      <c r="E74" s="59" t="s">
+      <c r="E74" s="58" t="s">
         <v>74</v>
       </c>
     </row>
@@ -3737,19 +3735,19 @@
         <f>D74-2*D68</f>
         <v>2.6951999999999998</v>
       </c>
-      <c r="E75" s="59" t="s">
+      <c r="E75" s="58" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="76" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C76" s="53" t="s">
+      <c r="C76" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="D76" s="54">
+      <c r="D76" s="53">
         <f>D75*100/D69</f>
         <v>53.903999999999996</v>
       </c>
-      <c r="E76" s="60" t="s">
+      <c r="E76" s="59" t="s">
         <v>80</v>
       </c>
     </row>
@@ -3765,20 +3763,20 @@
     </row>
     <row r="79" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="80" spans="3:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C80" s="95" t="s">
+      <c r="C80" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="D80" s="96"/>
-      <c r="E80" s="97"/>
+      <c r="D80" s="83"/>
+      <c r="E80" s="84"/>
     </row>
     <row r="81" spans="3:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C81" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D81" s="58" t="s">
+      <c r="D81" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="E81" s="66" t="s">
+      <c r="E81" s="65" t="s">
         <v>88</v>
       </c>
     </row>
@@ -3802,9 +3800,9 @@
     </row>
     <row r="87" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="88" spans="3:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C88" s="95"/>
-      <c r="D88" s="96"/>
-      <c r="E88" s="97"/>
+      <c r="C88" s="82"/>
+      <c r="D88" s="83"/>
+      <c r="E88" s="84"/>
     </row>
     <row r="89" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C89" s="2"/>
@@ -3813,327 +3811,309 @@
     </row>
     <row r="90" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C90" s="9"/>
-      <c r="D90" s="58"/>
+      <c r="D90" s="57"/>
       <c r="E90" s="11"/>
     </row>
     <row r="94" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="95" spans="3:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C95" s="95" t="s">
+      <c r="C95" s="82" t="s">
         <v>97</v>
       </c>
-      <c r="D95" s="96"/>
-      <c r="E95" s="97"/>
+      <c r="D95" s="83"/>
+      <c r="E95" s="84"/>
     </row>
     <row r="96" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C96" s="69" t="s">
+      <c r="C96" s="68" t="s">
         <v>99</v>
       </c>
-      <c r="D96" s="70"/>
-      <c r="E96" s="70"/>
-      <c r="F96" s="70"/>
-      <c r="G96" s="70"/>
-      <c r="H96" s="71"/>
-      <c r="I96" s="72"/>
-      <c r="J96" s="68"/>
+      <c r="D96" s="69"/>
+      <c r="E96" s="69"/>
+      <c r="F96" s="69"/>
+      <c r="G96" s="69"/>
+      <c r="H96" s="70"/>
+      <c r="I96" s="71"/>
+      <c r="J96" s="67"/>
     </row>
     <row r="97" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C97" s="73" t="s">
+      <c r="C97" s="72" t="s">
         <v>100</v>
       </c>
-      <c r="D97" s="74"/>
-      <c r="E97" s="74"/>
-      <c r="F97" s="74"/>
-      <c r="G97" s="74"/>
-      <c r="H97" s="74"/>
-      <c r="I97" s="75"/>
-      <c r="J97" s="68"/>
+      <c r="D97" s="73"/>
+      <c r="E97" s="73"/>
+      <c r="F97" s="73"/>
+      <c r="G97" s="73"/>
+      <c r="H97" s="73"/>
+      <c r="I97" s="74"/>
+      <c r="J97" s="67"/>
     </row>
     <row r="98" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C98" s="76" t="s">
+      <c r="C98" s="75" t="s">
         <v>101</v>
       </c>
-      <c r="D98" s="68" t="s">
+      <c r="D98" s="67" t="s">
         <v>102</v>
       </c>
-      <c r="E98" s="68" t="s">
+      <c r="E98" s="67" t="s">
         <v>103</v>
       </c>
-      <c r="F98" s="68" t="s">
+      <c r="F98" s="67" t="s">
         <v>104</v>
       </c>
-      <c r="G98" s="68" t="s">
+      <c r="G98" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="H98" s="68" t="s">
+      <c r="H98" s="67" t="s">
         <v>105</v>
       </c>
-      <c r="I98" s="77" t="s">
+      <c r="I98" s="76" t="s">
         <v>106</v>
       </c>
-      <c r="J98" s="68"/>
+      <c r="J98" s="67"/>
     </row>
     <row r="99" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C99" s="76">
+      <c r="C99" s="75">
         <v>1</v>
       </c>
-      <c r="D99" s="68">
+      <c r="D99" s="67">
         <v>80.066000000000003</v>
       </c>
-      <c r="E99" s="68">
+      <c r="E99" s="67">
         <v>2</v>
       </c>
-      <c r="F99" s="68">
+      <c r="F99" s="67">
         <v>5</v>
       </c>
-      <c r="G99" s="68">
+      <c r="G99" s="67">
         <v>0.4</v>
       </c>
-      <c r="H99" s="68">
+      <c r="H99" s="67">
         <v>0.104</v>
       </c>
-      <c r="I99" s="77">
+      <c r="I99" s="76">
         <v>0.26100000000000001</v>
       </c>
-      <c r="J99" s="68"/>
+      <c r="J99" s="67"/>
     </row>
     <row r="100" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C100" s="76">
+      <c r="C100" s="75">
         <v>2</v>
       </c>
-      <c r="D100" s="68">
+      <c r="D100" s="67">
         <v>80.066000000000003</v>
       </c>
-      <c r="E100" s="68">
+      <c r="E100" s="67">
         <v>2</v>
       </c>
-      <c r="F100" s="68">
+      <c r="F100" s="67">
         <v>5</v>
       </c>
-      <c r="G100" s="68">
+      <c r="G100" s="67">
         <v>0.4</v>
       </c>
-      <c r="H100" s="68">
+      <c r="H100" s="67">
         <v>0.104</v>
       </c>
-      <c r="I100" s="77">
+      <c r="I100" s="76">
         <v>0.26100000000000001</v>
       </c>
-      <c r="J100" s="68"/>
+      <c r="J100" s="67"/>
     </row>
     <row r="101" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C101" s="76">
+      <c r="C101" s="75">
         <v>3</v>
       </c>
-      <c r="D101" s="68">
+      <c r="D101" s="67">
         <v>80.066000000000003</v>
       </c>
-      <c r="E101" s="68">
+      <c r="E101" s="67">
         <v>2</v>
       </c>
-      <c r="F101" s="68">
+      <c r="F101" s="67">
         <v>5</v>
       </c>
-      <c r="G101" s="68">
+      <c r="G101" s="67">
         <v>0.2</v>
       </c>
-      <c r="H101" s="68">
+      <c r="H101" s="67">
         <v>0.104</v>
       </c>
-      <c r="I101" s="77">
+      <c r="I101" s="76">
         <v>0.52200000000000002</v>
       </c>
-      <c r="J101" s="68" t="s">
+      <c r="J101" s="67" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="102" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C102" s="76">
+      <c r="C102" s="75">
         <v>4</v>
       </c>
-      <c r="D102" s="68">
+      <c r="D102" s="67">
         <v>80.066000000000003</v>
       </c>
-      <c r="E102" s="68">
+      <c r="E102" s="67">
         <v>2</v>
       </c>
-      <c r="F102" s="68">
+      <c r="F102" s="67">
         <v>8</v>
       </c>
-      <c r="G102" s="68">
+      <c r="G102" s="67">
         <v>0.25</v>
       </c>
-      <c r="H102" s="68">
+      <c r="H102" s="67">
         <v>0.104</v>
       </c>
-      <c r="I102" s="77">
+      <c r="I102" s="76">
         <v>0.41699999999999998</v>
       </c>
-      <c r="J102" s="68"/>
+      <c r="J102" s="67"/>
     </row>
     <row r="103" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C103" s="76">
+      <c r="C103" s="75">
         <v>5</v>
       </c>
-      <c r="D103" s="68">
+      <c r="D103" s="67">
         <v>80.066000000000003</v>
       </c>
-      <c r="E103" s="68">
+      <c r="E103" s="67">
         <v>2</v>
       </c>
-      <c r="F103" s="68">
+      <c r="F103" s="67">
         <v>11</v>
       </c>
-      <c r="G103" s="68">
+      <c r="G103" s="67">
         <v>0.18181818199999999</v>
       </c>
-      <c r="H103" s="68">
+      <c r="H103" s="67">
         <v>0.104</v>
       </c>
-      <c r="I103" s="77">
+      <c r="I103" s="76">
         <v>0.57899999999999996</v>
       </c>
-      <c r="J103" s="68"/>
+      <c r="J103" s="67"/>
     </row>
     <row r="104" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C104" s="78">
+      <c r="C104" s="77">
         <v>6</v>
       </c>
-      <c r="D104" s="74">
+      <c r="D104" s="73">
         <v>80.066000000000003</v>
       </c>
-      <c r="E104" s="74">
+      <c r="E104" s="73">
         <v>2</v>
       </c>
-      <c r="F104" s="74" t="s">
+      <c r="F104" s="73" t="s">
         <v>111</v>
       </c>
-      <c r="G104" s="74" t="s">
+      <c r="G104" s="73" t="s">
         <v>110</v>
       </c>
-      <c r="H104" s="74">
+      <c r="H104" s="73">
         <v>0.104</v>
       </c>
-      <c r="I104" s="79" t="s">
+      <c r="I104" s="78" t="s">
         <v>108</v>
       </c>
-      <c r="J104" s="68"/>
+      <c r="J104" s="67"/>
     </row>
     <row r="105" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C105" s="78">
+      <c r="C105" s="77">
         <v>7</v>
       </c>
-      <c r="D105" s="74">
+      <c r="D105" s="73">
         <v>80.066000000000003</v>
       </c>
-      <c r="E105" s="74">
+      <c r="E105" s="73">
         <v>2</v>
       </c>
-      <c r="F105" s="74" t="s">
+      <c r="F105" s="73" t="s">
         <v>111</v>
       </c>
-      <c r="G105" s="74" t="s">
+      <c r="G105" s="73" t="s">
         <v>110</v>
       </c>
-      <c r="H105" s="74">
+      <c r="H105" s="73">
         <v>0.104</v>
       </c>
-      <c r="I105" s="79" t="s">
+      <c r="I105" s="78" t="s">
         <v>108</v>
       </c>
-      <c r="J105" s="68"/>
+      <c r="J105" s="67"/>
     </row>
     <row r="106" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C106" s="78">
+      <c r="C106" s="77">
         <v>8</v>
       </c>
-      <c r="D106" s="74">
+      <c r="D106" s="73">
         <v>80.066000000000003</v>
       </c>
-      <c r="E106" s="74">
+      <c r="E106" s="73">
         <v>2</v>
       </c>
-      <c r="F106" s="74" t="s">
+      <c r="F106" s="73" t="s">
         <v>111</v>
       </c>
-      <c r="G106" s="74" t="s">
+      <c r="G106" s="73" t="s">
         <v>110</v>
       </c>
-      <c r="H106" s="74">
+      <c r="H106" s="73">
         <v>0.104</v>
       </c>
-      <c r="I106" s="79" t="s">
+      <c r="I106" s="78" t="s">
         <v>108</v>
       </c>
-      <c r="J106" s="68"/>
+      <c r="J106" s="67"/>
     </row>
     <row r="107" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C107" s="78">
+      <c r="C107" s="77">
         <v>9</v>
       </c>
-      <c r="D107" s="74">
+      <c r="D107" s="73">
         <v>80.066000000000003</v>
       </c>
-      <c r="E107" s="74">
+      <c r="E107" s="73">
         <v>2</v>
       </c>
-      <c r="F107" s="74" t="s">
+      <c r="F107" s="73" t="s">
         <v>111</v>
       </c>
-      <c r="G107" s="74" t="s">
+      <c r="G107" s="73" t="s">
         <v>110</v>
       </c>
-      <c r="H107" s="74">
+      <c r="H107" s="73">
         <v>0.104</v>
       </c>
-      <c r="I107" s="79" t="s">
+      <c r="I107" s="78" t="s">
         <v>108</v>
       </c>
-      <c r="J107" s="68"/>
+      <c r="J107" s="67"/>
     </row>
     <row r="108" spans="3:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C108" s="80">
+      <c r="C108" s="79">
         <v>10</v>
       </c>
-      <c r="D108" s="81">
+      <c r="D108" s="80">
         <v>80.066000000000003</v>
       </c>
-      <c r="E108" s="81">
+      <c r="E108" s="80">
         <v>2</v>
       </c>
-      <c r="F108" s="81">
+      <c r="F108" s="80">
         <v>8.6</v>
       </c>
-      <c r="G108" s="81"/>
-      <c r="H108" s="81">
+      <c r="G108" s="80"/>
+      <c r="H108" s="80">
         <v>0.104</v>
       </c>
-      <c r="I108" s="82">
+      <c r="I108" s="81">
         <v>0.45300000000000001</v>
       </c>
-      <c r="J108" s="68" t="s">
+      <c r="J108" s="67" t="s">
         <v>109</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="C95:E95"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="C88:E88"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="C80:E80"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="G30:I30"/>
     <mergeCell ref="J37:Y37"/>
     <mergeCell ref="J49:S49"/>
     <mergeCell ref="C39:C43"/>
@@ -4148,6 +4128,24 @@
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="D59:E59"/>
     <mergeCell ref="D60:E60"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="C95:E95"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="C88:E88"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="C80:E80"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="F49:I49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
correct clearance vs hug height
</commit_message>
<xml_diff>
--- a/Studies/USMap_Doubleday_2024/SETUPS Description Complete_sil.xlsx
+++ b/Studies/USMap_Doubleday_2024/SETUPS Description Complete_sil.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tford\dev\InSPIRE\Studies\USMap_Doubleday_2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kdoubled/Documents/repos/Public_Github/InSPIRE/Studies/USMap_Doubleday_2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD32F2A-FF4E-44BF-BFD7-EC398CB41F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8064130D-CE88-2F4F-AE09-E17EF9589162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-4470" windowWidth="16440" windowHeight="28320" xr2:uid="{20F8F7F2-6405-4778-91BF-D0B7AC5935BA}"/>
+    <workbookView xWindow="1240" yWindow="3960" windowWidth="36080" windowHeight="21100" xr2:uid="{20F8F7F2-6405-4778-91BF-D0B7AC5935BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="113">
   <si>
     <t>Scenario</t>
   </si>
@@ -470,6 +470,9 @@
   </si>
   <si>
     <t>variable</t>
+  </si>
+  <si>
+    <t>Variable</t>
   </si>
 </sst>
 </file>
@@ -1022,6 +1025,36 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1043,37 +1076,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1498,37 +1501,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932A1107-9899-4DFE-A9E6-0ED2844D3F4A}">
   <dimension ref="B2:AA108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" customWidth="1"/>
-    <col min="8" max="8" width="25.5703125" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="7" max="7" width="20.5" customWidth="1"/>
+    <col min="8" max="8" width="25.5" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
-    <col min="15" max="15" width="13.28515625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="13.28515625" customWidth="1"/>
-    <col min="17" max="17" width="11.140625" customWidth="1"/>
-    <col min="18" max="18" width="13.85546875" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="13.33203125" customWidth="1"/>
+    <col min="17" max="17" width="11.1640625" customWidth="1"/>
+    <col min="18" max="18" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:21" ht="23" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="T2" s="91" t="s">
+      <c r="T2" s="88" t="s">
         <v>60</v>
       </c>
-      <c r="U2" s="91"/>
-    </row>
-    <row r="3" spans="2:21" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U2" s="88"/>
+    </row>
+    <row r="3" spans="2:21" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="23" t="s">
         <v>0</v>
       </c>
@@ -1588,7 +1591,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B4" s="2">
         <v>1</v>
       </c>
@@ -1643,7 +1646,7 @@
       <c r="T4" s="26"/>
       <c r="U4" s="3"/>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B5" s="5">
         <v>2</v>
       </c>
@@ -1694,7 +1697,7 @@
       </c>
       <c r="T5" s="27"/>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B6" s="5">
         <v>3</v>
       </c>
@@ -1745,7 +1748,7 @@
       </c>
       <c r="T6" s="27"/>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B7" s="5">
         <v>4</v>
       </c>
@@ -1796,7 +1799,7 @@
       </c>
       <c r="T7" s="27"/>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B8" s="5">
         <v>5</v>
       </c>
@@ -1847,7 +1850,7 @@
       </c>
       <c r="T8" s="27"/>
     </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B9" s="64" t="s">
         <v>96</v>
       </c>
@@ -1861,15 +1864,15 @@
       <c r="R9" s="6"/>
       <c r="T9" s="27"/>
     </row>
-    <row r="10" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="5">
         <v>6</v>
       </c>
       <c r="C10">
         <v>1.5</v>
       </c>
-      <c r="D10">
-        <v>1.5</v>
+      <c r="D10" t="s">
+        <v>112</v>
       </c>
       <c r="E10" s="31" t="s">
         <v>61</v>
@@ -1916,15 +1919,15 @@
       <c r="T10" s="27"/>
       <c r="U10" s="19"/>
     </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B11" s="5">
         <v>7</v>
       </c>
       <c r="C11">
         <v>2.4</v>
       </c>
-      <c r="D11">
-        <v>2.4</v>
+      <c r="D11" t="s">
+        <v>112</v>
       </c>
       <c r="E11" s="31" t="s">
         <v>61</v>
@@ -1971,15 +1974,15 @@
       <c r="T11" s="27"/>
       <c r="U11" s="19"/>
     </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B12" s="5">
         <v>8</v>
       </c>
       <c r="C12">
         <v>2.4</v>
       </c>
-      <c r="D12">
-        <v>2.4</v>
+      <c r="D12" t="s">
+        <v>112</v>
       </c>
       <c r="E12" s="31" t="s">
         <v>61</v>
@@ -2026,15 +2029,15 @@
       <c r="T12" s="27"/>
       <c r="U12" s="19"/>
     </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B13" s="5">
         <v>9</v>
       </c>
       <c r="C13">
         <v>1.5</v>
       </c>
-      <c r="D13">
-        <v>1.5</v>
+      <c r="D13" t="s">
+        <v>112</v>
       </c>
       <c r="E13" s="31" t="s">
         <v>61</v>
@@ -2081,7 +2084,7 @@
       <c r="T13" s="27"/>
       <c r="U13" s="19"/>
     </row>
-    <row r="14" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="9">
         <v>10</v>
       </c>
@@ -2089,7 +2092,7 @@
         <v>0.6</v>
       </c>
       <c r="D14" s="21">
-        <v>2</v>
+        <v>1.6</v>
       </c>
       <c r="E14" s="22">
         <v>8.6</v>
@@ -2139,8 +2142,8 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="16" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:21" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="15" t="s">
         <v>40</v>
       </c>
@@ -2154,7 +2157,7 @@
       <c r="J17" s="16"/>
       <c r="K17" s="17"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
@@ -2184,7 +2187,7 @@
       </c>
       <c r="K18" s="4"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" s="5">
         <v>2</v>
       </c>
@@ -2218,7 +2221,7 @@
       </c>
       <c r="K19" s="6"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B20" s="5">
         <v>2</v>
       </c>
@@ -2249,12 +2252,12 @@
       </c>
       <c r="K20" s="6"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" s="5"/>
       <c r="H21" s="33"/>
       <c r="K21" s="6"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" s="5"/>
       <c r="C22" t="s">
         <v>90</v>
@@ -2274,7 +2277,7 @@
       </c>
       <c r="K22" s="6"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B23" s="5"/>
       <c r="C23" t="s">
         <v>91</v>
@@ -2294,7 +2297,7 @@
       </c>
       <c r="K23" s="6"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B24" s="5"/>
       <c r="F24">
         <v>2</v>
@@ -2308,7 +2311,7 @@
       </c>
       <c r="K24" s="6"/>
     </row>
-    <row r="25" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -2327,8 +2330,8 @@
       <c r="J25" s="10"/>
       <c r="K25" s="11"/>
     </row>
-    <row r="26" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B27" s="12" t="s">
         <v>35</v>
       </c>
@@ -2336,13 +2339,13 @@
       <c r="D27" s="13"/>
       <c r="E27" s="13"/>
       <c r="F27" s="14"/>
-      <c r="G27" s="92" t="s">
+      <c r="G27" s="89" t="s">
         <v>39</v>
       </c>
-      <c r="H27" s="93"/>
-      <c r="I27" s="93"/>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H27" s="90"/>
+      <c r="I27" s="90"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B28" s="5" t="s">
         <v>33</v>
       </c>
@@ -2350,11 +2353,11 @@
         <v>8</v>
       </c>
       <c r="F28" s="6"/>
-      <c r="G28" s="94"/>
-      <c r="H28" s="89"/>
-      <c r="I28" s="89"/>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="G28" s="91"/>
+      <c r="H28" s="87"/>
+      <c r="I28" s="87"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B29" s="5" t="s">
         <v>32</v>
       </c>
@@ -2362,11 +2365,11 @@
         <v>2</v>
       </c>
       <c r="F29" s="6"/>
-      <c r="G29" s="94"/>
-      <c r="H29" s="89"/>
-      <c r="I29" s="89"/>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="G29" s="91"/>
+      <c r="H29" s="87"/>
+      <c r="I29" s="87"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B30" s="5" t="s">
         <v>24</v>
       </c>
@@ -2382,11 +2385,11 @@
       <c r="F30" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G30" s="94"/>
-      <c r="H30" s="89"/>
-      <c r="I30" s="89"/>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="G30" s="91"/>
+      <c r="H30" s="87"/>
+      <c r="I30" s="87"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B31" s="5" t="s">
         <v>36</v>
       </c>
@@ -2406,13 +2409,13 @@
         <f>ROUND(D31/10,0)</f>
         <v>3</v>
       </c>
-      <c r="G31" s="87" t="s">
+      <c r="G31" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="H31" s="88"/>
-      <c r="I31" s="88"/>
-    </row>
-    <row r="32" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H31" s="98"/>
+      <c r="I31" s="98"/>
+    </row>
+    <row r="32" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B32" s="9" t="s">
         <v>30</v>
       </c>
@@ -2432,46 +2435,46 @@
         <f>ROUND(D32/10,0)</f>
         <v>8</v>
       </c>
-      <c r="G32" s="87" t="s">
+      <c r="G32" s="97" t="s">
         <v>38</v>
       </c>
-      <c r="H32" s="88"/>
-      <c r="I32" s="88"/>
-    </row>
-    <row r="36" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="H32" s="98"/>
+      <c r="I32" s="98"/>
+    </row>
+    <row r="36" spans="3:26" x14ac:dyDescent="0.2">
       <c r="O36"/>
     </row>
-    <row r="37" spans="3:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="95"/>
+    <row r="37" spans="3:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C37" s="82"/>
       <c r="D37" s="35"/>
       <c r="E37" s="35"/>
-      <c r="F37" s="90" t="s">
+      <c r="F37" s="99" t="s">
         <v>59</v>
       </c>
-      <c r="G37" s="90"/>
-      <c r="H37" s="90"/>
-      <c r="I37" s="90"/>
-      <c r="J37" s="95" t="s">
+      <c r="G37" s="99"/>
+      <c r="H37" s="99"/>
+      <c r="I37" s="99"/>
+      <c r="J37" s="82" t="s">
         <v>58</v>
       </c>
-      <c r="K37" s="95"/>
-      <c r="L37" s="95"/>
-      <c r="M37" s="95"/>
-      <c r="N37" s="95"/>
-      <c r="O37" s="95"/>
-      <c r="P37" s="95"/>
-      <c r="Q37" s="95"/>
-      <c r="R37" s="95"/>
-      <c r="S37" s="95"/>
-      <c r="T37" s="95"/>
-      <c r="U37" s="95"/>
-      <c r="V37" s="95"/>
-      <c r="W37" s="95"/>
-      <c r="X37" s="95"/>
-      <c r="Y37" s="95"/>
-    </row>
-    <row r="38" spans="3:26" s="36" customFormat="1" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C38" s="95"/>
+      <c r="K37" s="82"/>
+      <c r="L37" s="82"/>
+      <c r="M37" s="82"/>
+      <c r="N37" s="82"/>
+      <c r="O37" s="82"/>
+      <c r="P37" s="82"/>
+      <c r="Q37" s="82"/>
+      <c r="R37" s="82"/>
+      <c r="S37" s="82"/>
+      <c r="T37" s="82"/>
+      <c r="U37" s="82"/>
+      <c r="V37" s="82"/>
+      <c r="W37" s="82"/>
+      <c r="X37" s="82"/>
+      <c r="Y37" s="82"/>
+    </row>
+    <row r="38" spans="3:26" s="36" customFormat="1" ht="25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C38" s="82"/>
       <c r="D38" s="37" t="s">
         <v>0</v>
       </c>
@@ -2542,8 +2545,8 @@
         <v>92</v>
       </c>
     </row>
-    <row r="39" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C39" s="96" t="s">
+    <row r="39" spans="3:26" x14ac:dyDescent="0.2">
+      <c r="C39" s="83" t="s">
         <v>66</v>
       </c>
       <c r="D39">
@@ -2595,8 +2598,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C40" s="96"/>
+    <row r="40" spans="3:26" x14ac:dyDescent="0.2">
+      <c r="C40" s="83"/>
       <c r="D40">
         <v>2</v>
       </c>
@@ -2646,8 +2649,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C41" s="96"/>
+    <row r="41" spans="3:26" x14ac:dyDescent="0.2">
+      <c r="C41" s="83"/>
       <c r="D41">
         <v>3</v>
       </c>
@@ -2697,8 +2700,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C42" s="96"/>
+    <row r="42" spans="3:26" x14ac:dyDescent="0.2">
+      <c r="C42" s="83"/>
       <c r="D42">
         <v>4</v>
       </c>
@@ -2748,8 +2751,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C43" s="96"/>
+    <row r="43" spans="3:26" x14ac:dyDescent="0.2">
+      <c r="C43" s="83"/>
       <c r="D43">
         <v>5</v>
       </c>
@@ -2817,7 +2820,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C44" s="50" t="s">
         <v>67</v>
       </c>
@@ -2888,55 +2891,55 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:26" x14ac:dyDescent="0.2">
       <c r="M45" s="1"/>
       <c r="O45"/>
     </row>
-    <row r="46" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:26" x14ac:dyDescent="0.2">
       <c r="M46" s="1"/>
       <c r="O46"/>
     </row>
-    <row r="47" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:26" x14ac:dyDescent="0.2">
       <c r="M47" s="1"/>
       <c r="O47"/>
     </row>
-    <row r="48" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:26" x14ac:dyDescent="0.2">
       <c r="M48" s="1"/>
       <c r="O48"/>
     </row>
-    <row r="49" spans="3:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C49" s="97" t="s">
+    <row r="49" spans="3:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C49" s="84" t="s">
         <v>68</v>
       </c>
-      <c r="D49" s="99" t="s">
+      <c r="D49" s="86" t="s">
         <v>62</v>
       </c>
-      <c r="E49" s="99"/>
-      <c r="F49" s="90" t="s">
+      <c r="E49" s="86"/>
+      <c r="F49" s="99" t="s">
         <v>59</v>
       </c>
-      <c r="G49" s="90"/>
-      <c r="H49" s="90"/>
-      <c r="I49" s="90"/>
-      <c r="J49" s="95" t="s">
+      <c r="G49" s="99"/>
+      <c r="H49" s="99"/>
+      <c r="I49" s="99"/>
+      <c r="J49" s="82" t="s">
         <v>58</v>
       </c>
-      <c r="K49" s="95"/>
-      <c r="L49" s="95"/>
-      <c r="M49" s="95"/>
-      <c r="N49" s="95"/>
-      <c r="O49" s="95"/>
-      <c r="P49" s="95"/>
-      <c r="Q49" s="95"/>
-      <c r="R49" s="95"/>
-      <c r="S49" s="95"/>
-    </row>
-    <row r="50" spans="3:19" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C50" s="97"/>
-      <c r="D50" s="98" t="s">
+      <c r="K49" s="82"/>
+      <c r="L49" s="82"/>
+      <c r="M49" s="82"/>
+      <c r="N49" s="82"/>
+      <c r="O49" s="82"/>
+      <c r="P49" s="82"/>
+      <c r="Q49" s="82"/>
+      <c r="R49" s="82"/>
+      <c r="S49" s="82"/>
+    </row>
+    <row r="50" spans="3:19" ht="25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C50" s="84"/>
+      <c r="D50" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="E50" s="98"/>
+      <c r="E50" s="85"/>
       <c r="F50" s="38" t="s">
         <v>57</v>
       </c>
@@ -2980,12 +2983,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="51" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C51" s="97"/>
-      <c r="D51" s="89">
+    <row r="51" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C51" s="84"/>
+      <c r="D51" s="87">
         <v>3.8</v>
       </c>
-      <c r="E51" s="89"/>
+      <c r="E51" s="87"/>
       <c r="F51">
         <v>0</v>
       </c>
@@ -3029,12 +3032,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C52" s="97"/>
-      <c r="D52" s="89">
+    <row r="52" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C52" s="84"/>
+      <c r="D52" s="87">
         <v>4</v>
       </c>
-      <c r="E52" s="89"/>
+      <c r="E52" s="87"/>
       <c r="F52">
         <v>0</v>
       </c>
@@ -3078,12 +3081,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="53" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C53" s="97"/>
-      <c r="D53" s="89">
+    <row r="53" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C53" s="84"/>
+      <c r="D53" s="87">
         <v>4.5</v>
       </c>
-      <c r="E53" s="89"/>
+      <c r="E53" s="87"/>
       <c r="F53">
         <v>0</v>
       </c>
@@ -3127,12 +3130,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C54" s="97"/>
-      <c r="D54" s="89">
+    <row r="54" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C54" s="84"/>
+      <c r="D54" s="87">
         <v>5</v>
       </c>
-      <c r="E54" s="89"/>
+      <c r="E54" s="87"/>
       <c r="F54">
         <v>0</v>
       </c>
@@ -3176,12 +3179,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="55" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C55" s="97"/>
-      <c r="D55" s="89">
+    <row r="55" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C55" s="84"/>
+      <c r="D55" s="87">
         <v>5.5</v>
       </c>
-      <c r="E55" s="89"/>
+      <c r="E55" s="87"/>
       <c r="F55">
         <v>0</v>
       </c>
@@ -3225,12 +3228,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C56" s="97"/>
-      <c r="D56" s="89">
+    <row r="56" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C56" s="84"/>
+      <c r="D56" s="87">
         <v>6</v>
       </c>
-      <c r="E56" s="89"/>
+      <c r="E56" s="87"/>
       <c r="F56">
         <v>0</v>
       </c>
@@ -3274,12 +3277,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="57" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C57" s="97"/>
-      <c r="D57" s="89">
+    <row r="57" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C57" s="84"/>
+      <c r="D57" s="87">
         <v>6.5</v>
       </c>
-      <c r="E57" s="89"/>
+      <c r="E57" s="87"/>
       <c r="F57">
         <v>0</v>
       </c>
@@ -3323,12 +3326,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="58" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C58" s="97"/>
-      <c r="D58" s="89">
+    <row r="58" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C58" s="84"/>
+      <c r="D58" s="87">
         <v>7</v>
       </c>
-      <c r="E58" s="89"/>
+      <c r="E58" s="87"/>
       <c r="F58">
         <v>0</v>
       </c>
@@ -3372,12 +3375,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="59" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C59" s="97"/>
-      <c r="D59" s="89">
+    <row r="59" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C59" s="84"/>
+      <c r="D59" s="87">
         <v>7.5</v>
       </c>
-      <c r="E59" s="89"/>
+      <c r="E59" s="87"/>
       <c r="F59">
         <v>0</v>
       </c>
@@ -3421,12 +3424,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="60" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C60" s="97"/>
-      <c r="D60" s="89">
+    <row r="60" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C60" s="84"/>
+      <c r="D60" s="87">
         <v>8</v>
       </c>
-      <c r="E60" s="89"/>
+      <c r="E60" s="87"/>
       <c r="F60">
         <v>0</v>
       </c>
@@ -3470,12 +3473,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="61" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C61" s="97"/>
-      <c r="D61" s="89">
+    <row r="61" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C61" s="84"/>
+      <c r="D61" s="87">
         <v>8.5</v>
       </c>
-      <c r="E61" s="89"/>
+      <c r="E61" s="87"/>
       <c r="F61">
         <v>0</v>
       </c>
@@ -3519,12 +3522,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="62" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C62" s="97"/>
-      <c r="D62" s="89">
+    <row r="62" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C62" s="84"/>
+      <c r="D62" s="87">
         <v>9</v>
       </c>
-      <c r="E62" s="89"/>
+      <c r="E62" s="87"/>
       <c r="F62">
         <v>0</v>
       </c>
@@ -3568,7 +3571,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="63" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:19" x14ac:dyDescent="0.2">
       <c r="D63" t="s">
         <v>64</v>
       </c>
@@ -3615,15 +3618,15 @@
         <v>44</v>
       </c>
     </row>
-    <row r="64" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:19" x14ac:dyDescent="0.2">
       <c r="M64" s="1"/>
       <c r="O64"/>
     </row>
-    <row r="65" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="N65" s="1"/>
       <c r="O65"/>
     </row>
-    <row r="66" spans="3:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="3:27" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C66" s="54" t="s">
         <v>69</v>
       </c>
@@ -3632,17 +3635,17 @@
       <c r="O66"/>
       <c r="AA66" s="1"/>
     </row>
-    <row r="67" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C67" s="5" t="s">
         <v>73</v>
       </c>
       <c r="E67" s="58"/>
-      <c r="F67" s="85" t="s">
+      <c r="F67" s="95" t="s">
         <v>95</v>
       </c>
-      <c r="G67" s="86"/>
-    </row>
-    <row r="68" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G67" s="96"/>
+    </row>
+    <row r="68" spans="3:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C68" s="5" t="s">
         <v>70</v>
       </c>
@@ -3660,7 +3663,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="69" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C69" s="5" t="s">
         <v>72</v>
       </c>
@@ -3671,7 +3674,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="70" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C70" s="5" t="s">
         <v>23</v>
       </c>
@@ -3682,7 +3685,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="71" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C71" s="5" t="s">
         <v>24</v>
       </c>
@@ -3693,7 +3696,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="72" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C72" s="5" t="s">
         <v>17</v>
       </c>
@@ -3703,7 +3706,7 @@
       </c>
       <c r="E72" s="58"/>
     </row>
-    <row r="73" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C73" s="5" t="s">
         <v>77</v>
       </c>
@@ -3715,7 +3718,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="74" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C74" s="5" t="s">
         <v>76</v>
       </c>
@@ -3727,7 +3730,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C75" s="5" t="s">
         <v>75</v>
       </c>
@@ -3739,7 +3742,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="3:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C76" s="52" t="s">
         <v>79</v>
       </c>
@@ -3751,25 +3754,25 @@
         <v>80</v>
       </c>
     </row>
-    <row r="77" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C77" s="5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="78" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C78" s="5" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="79" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="80" spans="3:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C80" s="82" t="s">
+    <row r="79" spans="3:27" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="3:27" ht="19" x14ac:dyDescent="0.25">
+      <c r="C80" s="92" t="s">
         <v>82</v>
       </c>
-      <c r="D80" s="83"/>
-      <c r="E80" s="84"/>
-    </row>
-    <row r="81" spans="3:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D80" s="93"/>
+      <c r="E80" s="94"/>
+    </row>
+    <row r="81" spans="3:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C81" s="9" t="s">
         <v>84</v>
       </c>
@@ -3780,17 +3783,17 @@
         <v>88</v>
       </c>
     </row>
-    <row r="83" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C83" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="84" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C84" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="85" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C85" t="s">
         <v>87</v>
       </c>
@@ -3798,31 +3801,31 @@
         <v>83</v>
       </c>
     </row>
-    <row r="87" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="88" spans="3:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C88" s="82"/>
-      <c r="D88" s="83"/>
-      <c r="E88" s="84"/>
-    </row>
-    <row r="89" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="88" spans="3:10" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C88" s="92"/>
+      <c r="D88" s="93"/>
+      <c r="E88" s="94"/>
+    </row>
+    <row r="89" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C89" s="2"/>
       <c r="D89" s="3"/>
       <c r="E89" s="4"/>
     </row>
-    <row r="90" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="3:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C90" s="9"/>
       <c r="D90" s="57"/>
       <c r="E90" s="11"/>
     </row>
-    <row r="94" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="95" spans="3:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C95" s="82" t="s">
+    <row r="94" spans="3:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="95" spans="3:10" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C95" s="92" t="s">
         <v>97</v>
       </c>
-      <c r="D95" s="83"/>
-      <c r="E95" s="84"/>
-    </row>
-    <row r="96" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D95" s="93"/>
+      <c r="E95" s="94"/>
+    </row>
+    <row r="96" spans="3:10" ht="16" x14ac:dyDescent="0.2">
       <c r="C96" s="68" t="s">
         <v>99</v>
       </c>
@@ -3834,7 +3837,7 @@
       <c r="I96" s="71"/>
       <c r="J96" s="67"/>
     </row>
-    <row r="97" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:10" ht="16" x14ac:dyDescent="0.2">
       <c r="C97" s="72" t="s">
         <v>100</v>
       </c>
@@ -3846,7 +3849,7 @@
       <c r="I97" s="74"/>
       <c r="J97" s="67"/>
     </row>
-    <row r="98" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:10" ht="16" x14ac:dyDescent="0.2">
       <c r="C98" s="75" t="s">
         <v>101</v>
       </c>
@@ -3870,7 +3873,7 @@
       </c>
       <c r="J98" s="67"/>
     </row>
-    <row r="99" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:10" ht="16" x14ac:dyDescent="0.2">
       <c r="C99" s="75">
         <v>1</v>
       </c>
@@ -3894,7 +3897,7 @@
       </c>
       <c r="J99" s="67"/>
     </row>
-    <row r="100" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:10" ht="16" x14ac:dyDescent="0.2">
       <c r="C100" s="75">
         <v>2</v>
       </c>
@@ -3918,7 +3921,7 @@
       </c>
       <c r="J100" s="67"/>
     </row>
-    <row r="101" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:10" ht="16" x14ac:dyDescent="0.2">
       <c r="C101" s="75">
         <v>3</v>
       </c>
@@ -3944,7 +3947,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="102" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:10" ht="16" x14ac:dyDescent="0.2">
       <c r="C102" s="75">
         <v>4</v>
       </c>
@@ -3968,7 +3971,7 @@
       </c>
       <c r="J102" s="67"/>
     </row>
-    <row r="103" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:10" ht="16" x14ac:dyDescent="0.2">
       <c r="C103" s="75">
         <v>5</v>
       </c>
@@ -3992,7 +3995,7 @@
       </c>
       <c r="J103" s="67"/>
     </row>
-    <row r="104" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:10" ht="16" x14ac:dyDescent="0.2">
       <c r="C104" s="77">
         <v>6</v>
       </c>
@@ -4016,7 +4019,7 @@
       </c>
       <c r="J104" s="67"/>
     </row>
-    <row r="105" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:10" ht="16" x14ac:dyDescent="0.2">
       <c r="C105" s="77">
         <v>7</v>
       </c>
@@ -4040,7 +4043,7 @@
       </c>
       <c r="J105" s="67"/>
     </row>
-    <row r="106" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:10" ht="16" x14ac:dyDescent="0.2">
       <c r="C106" s="77">
         <v>8</v>
       </c>
@@ -4064,7 +4067,7 @@
       </c>
       <c r="J106" s="67"/>
     </row>
-    <row r="107" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:10" ht="16" x14ac:dyDescent="0.2">
       <c r="C107" s="77">
         <v>9</v>
       </c>
@@ -4088,7 +4091,7 @@
       </c>
       <c r="J107" s="67"/>
     </row>
-    <row r="108" spans="3:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C108" s="79">
         <v>10</v>
       </c>
@@ -4114,6 +4117,24 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="C95:E95"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="C88:E88"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="C80:E80"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="G30:I30"/>
     <mergeCell ref="J37:Y37"/>
     <mergeCell ref="J49:S49"/>
     <mergeCell ref="C39:C43"/>
@@ -4128,24 +4149,6 @@
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="D59:E59"/>
     <mergeCell ref="D60:E60"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="C95:E95"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="C88:E88"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="C80:E80"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="F49:I49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Bin Sizing Added to SETUPS
</commit_message>
<xml_diff>
--- a/Studies/USMap_Doubleday_2024/SETUPS Description Complete_sil.xlsx
+++ b/Studies/USMap_Doubleday_2024/SETUPS Description Complete_sil.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kdoubled/Documents/repos/Public_Github/InSPIRE/Studies/USMap_Doubleday_2024/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sayala\Documents\GitHub\InSPIRE\Studies\USMap_Doubleday_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8064130D-CE88-2F4F-AE09-E17EF9589162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C63782A-EF3E-4622-A677-DA026DAEC16A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1240" yWindow="3960" windowWidth="36080" windowHeight="21100" xr2:uid="{20F8F7F2-6405-4778-91BF-D0B7AC5935BA}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{20F8F7F2-6405-4778-91BF-D0B7AC5935BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="122">
   <si>
     <t>Scenario</t>
   </si>
@@ -473,6 +473,33 @@
   </si>
   <si>
     <t>Variable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pitch </t>
+  </si>
+  <si>
+    <t>Bins</t>
+  </si>
+  <si>
+    <t>Bin Size</t>
+  </si>
+  <si>
+    <t>BINS</t>
+  </si>
+  <si>
+    <t>Module Length</t>
+  </si>
+  <si>
+    <t>GCR = CW / pitch</t>
+  </si>
+  <si>
+    <t>Bin End</t>
+  </si>
+  <si>
+    <t>Bin Start</t>
+  </si>
+  <si>
+    <t>Bin center location</t>
   </si>
 </sst>
 </file>
@@ -622,7 +649,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -731,8 +758,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -872,11 +905,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1025,6 +1138,45 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1040,43 +1192,33 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1499,39 +1641,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932A1107-9899-4DFE-A9E6-0ED2844D3F4A}">
-  <dimension ref="B2:AA108"/>
+  <dimension ref="B2:AA122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="A98" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B122" sqref="B122"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="21.83203125" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" customWidth="1"/>
-    <col min="6" max="6" width="14.5" customWidth="1"/>
-    <col min="7" max="7" width="20.5" customWidth="1"/>
-    <col min="8" max="8" width="25.5" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
-    <col min="15" max="15" width="13.33203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="13.33203125" customWidth="1"/>
-    <col min="17" max="17" width="11.1640625" customWidth="1"/>
-    <col min="18" max="18" width="13.83203125" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="13.28515625" customWidth="1"/>
+    <col min="17" max="17" width="11.140625" customWidth="1"/>
+    <col min="18" max="18" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:21" ht="23" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="T2" s="88" t="s">
+      <c r="T2" s="91" t="s">
         <v>60</v>
       </c>
-      <c r="U2" s="88"/>
-    </row>
-    <row r="3" spans="2:21" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U2" s="91"/>
+    </row>
+    <row r="3" spans="2:21" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="23" t="s">
         <v>0</v>
       </c>
@@ -1591,7 +1733,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>1</v>
       </c>
@@ -1646,7 +1788,7 @@
       <c r="T4" s="26"/>
       <c r="U4" s="3"/>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B5" s="5">
         <v>2</v>
       </c>
@@ -1697,7 +1839,7 @@
       </c>
       <c r="T5" s="27"/>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B6" s="5">
         <v>3</v>
       </c>
@@ -1748,7 +1890,7 @@
       </c>
       <c r="T6" s="27"/>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B7" s="5">
         <v>4</v>
       </c>
@@ -1799,7 +1941,7 @@
       </c>
       <c r="T7" s="27"/>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B8" s="5">
         <v>5</v>
       </c>
@@ -1850,7 +1992,7 @@
       </c>
       <c r="T8" s="27"/>
     </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B9" s="64" t="s">
         <v>96</v>
       </c>
@@ -1864,7 +2006,7 @@
       <c r="R9" s="6"/>
       <c r="T9" s="27"/>
     </row>
-    <row r="10" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
         <v>6</v>
       </c>
@@ -1919,7 +2061,7 @@
       <c r="T10" s="27"/>
       <c r="U10" s="19"/>
     </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B11" s="5">
         <v>7</v>
       </c>
@@ -1974,7 +2116,7 @@
       <c r="T11" s="27"/>
       <c r="U11" s="19"/>
     </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B12" s="5">
         <v>8</v>
       </c>
@@ -2029,7 +2171,7 @@
       <c r="T12" s="27"/>
       <c r="U12" s="19"/>
     </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B13" s="5">
         <v>9</v>
       </c>
@@ -2084,7 +2226,7 @@
       <c r="T13" s="27"/>
       <c r="U13" s="19"/>
     </row>
-    <row r="14" spans="2:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="9">
         <v>10</v>
       </c>
@@ -2142,8 +2284,8 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="16" spans="2:21" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="15" t="s">
         <v>40</v>
       </c>
@@ -2157,7 +2299,7 @@
       <c r="J17" s="16"/>
       <c r="K17" s="17"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
@@ -2187,7 +2329,7 @@
       </c>
       <c r="K18" s="4"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="5">
         <v>2</v>
       </c>
@@ -2221,7 +2363,7 @@
       </c>
       <c r="K19" s="6"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="5">
         <v>2</v>
       </c>
@@ -2252,12 +2394,12 @@
       </c>
       <c r="K20" s="6"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
       <c r="H21" s="33"/>
       <c r="K21" s="6"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
       <c r="C22" t="s">
         <v>90</v>
@@ -2277,7 +2419,7 @@
       </c>
       <c r="K22" s="6"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
       <c r="C23" t="s">
         <v>91</v>
@@ -2297,7 +2439,7 @@
       </c>
       <c r="K23" s="6"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
       <c r="F24">
         <v>2</v>
@@ -2311,7 +2453,7 @@
       </c>
       <c r="K24" s="6"/>
     </row>
-    <row r="25" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="9"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -2330,8 +2472,8 @@
       <c r="J25" s="10"/>
       <c r="K25" s="11"/>
     </row>
-    <row r="26" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="12" t="s">
         <v>35</v>
       </c>
@@ -2339,13 +2481,13 @@
       <c r="D27" s="13"/>
       <c r="E27" s="13"/>
       <c r="F27" s="14"/>
-      <c r="G27" s="89" t="s">
+      <c r="G27" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="H27" s="90"/>
-      <c r="I27" s="90"/>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="H27" s="93"/>
+      <c r="I27" s="93"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>33</v>
       </c>
@@ -2353,11 +2495,11 @@
         <v>8</v>
       </c>
       <c r="F28" s="6"/>
-      <c r="G28" s="91"/>
-      <c r="H28" s="87"/>
-      <c r="I28" s="87"/>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="G28" s="94"/>
+      <c r="H28" s="89"/>
+      <c r="I28" s="89"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>32</v>
       </c>
@@ -2365,11 +2507,11 @@
         <v>2</v>
       </c>
       <c r="F29" s="6"/>
-      <c r="G29" s="91"/>
-      <c r="H29" s="87"/>
-      <c r="I29" s="87"/>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="G29" s="94"/>
+      <c r="H29" s="89"/>
+      <c r="I29" s="89"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>24</v>
       </c>
@@ -2385,11 +2527,11 @@
       <c r="F30" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G30" s="91"/>
-      <c r="H30" s="87"/>
-      <c r="I30" s="87"/>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="G30" s="94"/>
+      <c r="H30" s="89"/>
+      <c r="I30" s="89"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>36</v>
       </c>
@@ -2409,13 +2551,13 @@
         <f>ROUND(D31/10,0)</f>
         <v>3</v>
       </c>
-      <c r="G31" s="97" t="s">
+      <c r="G31" s="87" t="s">
         <v>37</v>
       </c>
-      <c r="H31" s="98"/>
-      <c r="I31" s="98"/>
-    </row>
-    <row r="32" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H31" s="88"/>
+      <c r="I31" s="88"/>
+    </row>
+    <row r="32" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="9" t="s">
         <v>30</v>
       </c>
@@ -2435,46 +2577,46 @@
         <f>ROUND(D32/10,0)</f>
         <v>8</v>
       </c>
-      <c r="G32" s="97" t="s">
+      <c r="G32" s="87" t="s">
         <v>38</v>
       </c>
-      <c r="H32" s="98"/>
-      <c r="I32" s="98"/>
-    </row>
-    <row r="36" spans="3:26" x14ac:dyDescent="0.2">
+      <c r="H32" s="88"/>
+      <c r="I32" s="88"/>
+    </row>
+    <row r="36" spans="3:26" x14ac:dyDescent="0.25">
       <c r="O36"/>
     </row>
-    <row r="37" spans="3:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C37" s="82"/>
+    <row r="37" spans="3:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C37" s="95"/>
       <c r="D37" s="35"/>
       <c r="E37" s="35"/>
-      <c r="F37" s="99" t="s">
+      <c r="F37" s="90" t="s">
         <v>59</v>
       </c>
-      <c r="G37" s="99"/>
-      <c r="H37" s="99"/>
-      <c r="I37" s="99"/>
-      <c r="J37" s="82" t="s">
+      <c r="G37" s="90"/>
+      <c r="H37" s="90"/>
+      <c r="I37" s="90"/>
+      <c r="J37" s="95" t="s">
         <v>58</v>
       </c>
-      <c r="K37" s="82"/>
-      <c r="L37" s="82"/>
-      <c r="M37" s="82"/>
-      <c r="N37" s="82"/>
-      <c r="O37" s="82"/>
-      <c r="P37" s="82"/>
-      <c r="Q37" s="82"/>
-      <c r="R37" s="82"/>
-      <c r="S37" s="82"/>
-      <c r="T37" s="82"/>
-      <c r="U37" s="82"/>
-      <c r="V37" s="82"/>
-      <c r="W37" s="82"/>
-      <c r="X37" s="82"/>
-      <c r="Y37" s="82"/>
-    </row>
-    <row r="38" spans="3:26" s="36" customFormat="1" ht="25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="82"/>
+      <c r="K37" s="95"/>
+      <c r="L37" s="95"/>
+      <c r="M37" s="95"/>
+      <c r="N37" s="95"/>
+      <c r="O37" s="95"/>
+      <c r="P37" s="95"/>
+      <c r="Q37" s="95"/>
+      <c r="R37" s="95"/>
+      <c r="S37" s="95"/>
+      <c r="T37" s="95"/>
+      <c r="U37" s="95"/>
+      <c r="V37" s="95"/>
+      <c r="W37" s="95"/>
+      <c r="X37" s="95"/>
+      <c r="Y37" s="95"/>
+    </row>
+    <row r="38" spans="3:26" s="36" customFormat="1" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C38" s="95"/>
       <c r="D38" s="37" t="s">
         <v>0</v>
       </c>
@@ -2545,8 +2687,8 @@
         <v>92</v>
       </c>
     </row>
-    <row r="39" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="C39" s="83" t="s">
+    <row r="39" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C39" s="96" t="s">
         <v>66</v>
       </c>
       <c r="D39">
@@ -2598,8 +2740,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="C40" s="83"/>
+    <row r="40" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C40" s="96"/>
       <c r="D40">
         <v>2</v>
       </c>
@@ -2649,8 +2791,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="C41" s="83"/>
+    <row r="41" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C41" s="96"/>
       <c r="D41">
         <v>3</v>
       </c>
@@ -2700,8 +2842,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="C42" s="83"/>
+    <row r="42" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C42" s="96"/>
       <c r="D42">
         <v>4</v>
       </c>
@@ -2751,8 +2893,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="C43" s="83"/>
+    <row r="43" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C43" s="96"/>
       <c r="D43">
         <v>5</v>
       </c>
@@ -2820,7 +2962,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C44" s="50" t="s">
         <v>67</v>
       </c>
@@ -2891,55 +3033,55 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="45" spans="3:26" x14ac:dyDescent="0.25">
       <c r="M45" s="1"/>
       <c r="O45"/>
     </row>
-    <row r="46" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="46" spans="3:26" x14ac:dyDescent="0.25">
       <c r="M46" s="1"/>
       <c r="O46"/>
     </row>
-    <row r="47" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="47" spans="3:26" x14ac:dyDescent="0.25">
       <c r="M47" s="1"/>
       <c r="O47"/>
     </row>
-    <row r="48" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="48" spans="3:26" x14ac:dyDescent="0.25">
       <c r="M48" s="1"/>
       <c r="O48"/>
     </row>
-    <row r="49" spans="3:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C49" s="84" t="s">
+    <row r="49" spans="3:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C49" s="97" t="s">
         <v>68</v>
       </c>
-      <c r="D49" s="86" t="s">
+      <c r="D49" s="99" t="s">
         <v>62</v>
       </c>
-      <c r="E49" s="86"/>
-      <c r="F49" s="99" t="s">
+      <c r="E49" s="99"/>
+      <c r="F49" s="90" t="s">
         <v>59</v>
       </c>
-      <c r="G49" s="99"/>
-      <c r="H49" s="99"/>
-      <c r="I49" s="99"/>
-      <c r="J49" s="82" t="s">
+      <c r="G49" s="90"/>
+      <c r="H49" s="90"/>
+      <c r="I49" s="90"/>
+      <c r="J49" s="95" t="s">
         <v>58</v>
       </c>
-      <c r="K49" s="82"/>
-      <c r="L49" s="82"/>
-      <c r="M49" s="82"/>
-      <c r="N49" s="82"/>
-      <c r="O49" s="82"/>
-      <c r="P49" s="82"/>
-      <c r="Q49" s="82"/>
-      <c r="R49" s="82"/>
-      <c r="S49" s="82"/>
-    </row>
-    <row r="50" spans="3:19" ht="25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C50" s="84"/>
-      <c r="D50" s="85" t="s">
+      <c r="K49" s="95"/>
+      <c r="L49" s="95"/>
+      <c r="M49" s="95"/>
+      <c r="N49" s="95"/>
+      <c r="O49" s="95"/>
+      <c r="P49" s="95"/>
+      <c r="Q49" s="95"/>
+      <c r="R49" s="95"/>
+      <c r="S49" s="95"/>
+    </row>
+    <row r="50" spans="3:19" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C50" s="97"/>
+      <c r="D50" s="98" t="s">
         <v>63</v>
       </c>
-      <c r="E50" s="85"/>
+      <c r="E50" s="98"/>
       <c r="F50" s="38" t="s">
         <v>57</v>
       </c>
@@ -2983,12 +3125,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="51" spans="3:19" x14ac:dyDescent="0.2">
-      <c r="C51" s="84"/>
-      <c r="D51" s="87">
+    <row r="51" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C51" s="97"/>
+      <c r="D51" s="89">
         <v>3.8</v>
       </c>
-      <c r="E51" s="87"/>
+      <c r="E51" s="89"/>
       <c r="F51">
         <v>0</v>
       </c>
@@ -3032,12 +3174,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="3:19" x14ac:dyDescent="0.2">
-      <c r="C52" s="84"/>
-      <c r="D52" s="87">
+    <row r="52" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C52" s="97"/>
+      <c r="D52" s="89">
         <v>4</v>
       </c>
-      <c r="E52" s="87"/>
+      <c r="E52" s="89"/>
       <c r="F52">
         <v>0</v>
       </c>
@@ -3081,12 +3223,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="53" spans="3:19" x14ac:dyDescent="0.2">
-      <c r="C53" s="84"/>
-      <c r="D53" s="87">
+    <row r="53" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C53" s="97"/>
+      <c r="D53" s="89">
         <v>4.5</v>
       </c>
-      <c r="E53" s="87"/>
+      <c r="E53" s="89"/>
       <c r="F53">
         <v>0</v>
       </c>
@@ -3130,12 +3272,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="3:19" x14ac:dyDescent="0.2">
-      <c r="C54" s="84"/>
-      <c r="D54" s="87">
+    <row r="54" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C54" s="97"/>
+      <c r="D54" s="89">
         <v>5</v>
       </c>
-      <c r="E54" s="87"/>
+      <c r="E54" s="89"/>
       <c r="F54">
         <v>0</v>
       </c>
@@ -3179,12 +3321,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="55" spans="3:19" x14ac:dyDescent="0.2">
-      <c r="C55" s="84"/>
-      <c r="D55" s="87">
+    <row r="55" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C55" s="97"/>
+      <c r="D55" s="89">
         <v>5.5</v>
       </c>
-      <c r="E55" s="87"/>
+      <c r="E55" s="89"/>
       <c r="F55">
         <v>0</v>
       </c>
@@ -3228,12 +3370,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="3:19" x14ac:dyDescent="0.2">
-      <c r="C56" s="84"/>
-      <c r="D56" s="87">
+    <row r="56" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C56" s="97"/>
+      <c r="D56" s="89">
         <v>6</v>
       </c>
-      <c r="E56" s="87"/>
+      <c r="E56" s="89"/>
       <c r="F56">
         <v>0</v>
       </c>
@@ -3277,12 +3419,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="57" spans="3:19" x14ac:dyDescent="0.2">
-      <c r="C57" s="84"/>
-      <c r="D57" s="87">
+    <row r="57" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C57" s="97"/>
+      <c r="D57" s="89">
         <v>6.5</v>
       </c>
-      <c r="E57" s="87"/>
+      <c r="E57" s="89"/>
       <c r="F57">
         <v>0</v>
       </c>
@@ -3326,12 +3468,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="58" spans="3:19" x14ac:dyDescent="0.2">
-      <c r="C58" s="84"/>
-      <c r="D58" s="87">
+    <row r="58" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C58" s="97"/>
+      <c r="D58" s="89">
         <v>7</v>
       </c>
-      <c r="E58" s="87"/>
+      <c r="E58" s="89"/>
       <c r="F58">
         <v>0</v>
       </c>
@@ -3375,12 +3517,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="59" spans="3:19" x14ac:dyDescent="0.2">
-      <c r="C59" s="84"/>
-      <c r="D59" s="87">
+    <row r="59" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C59" s="97"/>
+      <c r="D59" s="89">
         <v>7.5</v>
       </c>
-      <c r="E59" s="87"/>
+      <c r="E59" s="89"/>
       <c r="F59">
         <v>0</v>
       </c>
@@ -3424,12 +3566,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="60" spans="3:19" x14ac:dyDescent="0.2">
-      <c r="C60" s="84"/>
-      <c r="D60" s="87">
+    <row r="60" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C60" s="97"/>
+      <c r="D60" s="89">
         <v>8</v>
       </c>
-      <c r="E60" s="87"/>
+      <c r="E60" s="89"/>
       <c r="F60">
         <v>0</v>
       </c>
@@ -3473,12 +3615,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="61" spans="3:19" x14ac:dyDescent="0.2">
-      <c r="C61" s="84"/>
-      <c r="D61" s="87">
+    <row r="61" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C61" s="97"/>
+      <c r="D61" s="89">
         <v>8.5</v>
       </c>
-      <c r="E61" s="87"/>
+      <c r="E61" s="89"/>
       <c r="F61">
         <v>0</v>
       </c>
@@ -3522,12 +3664,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="62" spans="3:19" x14ac:dyDescent="0.2">
-      <c r="C62" s="84"/>
-      <c r="D62" s="87">
+    <row r="62" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C62" s="97"/>
+      <c r="D62" s="89">
         <v>9</v>
       </c>
-      <c r="E62" s="87"/>
+      <c r="E62" s="89"/>
       <c r="F62">
         <v>0</v>
       </c>
@@ -3571,7 +3713,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="63" spans="3:19" x14ac:dyDescent="0.2">
+    <row r="63" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D63" t="s">
         <v>64</v>
       </c>
@@ -3618,15 +3760,15 @@
         <v>44</v>
       </c>
     </row>
-    <row r="64" spans="3:19" x14ac:dyDescent="0.2">
+    <row r="64" spans="3:19" x14ac:dyDescent="0.25">
       <c r="M64" s="1"/>
       <c r="O64"/>
     </row>
-    <row r="65" spans="3:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N65" s="1"/>
       <c r="O65"/>
     </row>
-    <row r="66" spans="3:27" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C66" s="54" t="s">
         <v>69</v>
       </c>
@@ -3635,17 +3777,17 @@
       <c r="O66"/>
       <c r="AA66" s="1"/>
     </row>
-    <row r="67" spans="3:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C67" s="5" t="s">
         <v>73</v>
       </c>
       <c r="E67" s="58"/>
-      <c r="F67" s="95" t="s">
+      <c r="F67" s="85" t="s">
         <v>95</v>
       </c>
-      <c r="G67" s="96"/>
-    </row>
-    <row r="68" spans="3:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G67" s="86"/>
+    </row>
+    <row r="68" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C68" s="5" t="s">
         <v>70</v>
       </c>
@@ -3663,7 +3805,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="69" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="69" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C69" s="5" t="s">
         <v>72</v>
       </c>
@@ -3674,7 +3816,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="70" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="70" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C70" s="5" t="s">
         <v>23</v>
       </c>
@@ -3685,7 +3827,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="71" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="71" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C71" s="5" t="s">
         <v>24</v>
       </c>
@@ -3696,7 +3838,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="72" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="72" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C72" s="5" t="s">
         <v>17</v>
       </c>
@@ -3706,7 +3848,7 @@
       </c>
       <c r="E72" s="58"/>
     </row>
-    <row r="73" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="73" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C73" s="5" t="s">
         <v>77</v>
       </c>
@@ -3718,7 +3860,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="74" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="74" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C74" s="5" t="s">
         <v>76</v>
       </c>
@@ -3730,7 +3872,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="75" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C75" s="5" t="s">
         <v>75</v>
       </c>
@@ -3742,7 +3884,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="3:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C76" s="52" t="s">
         <v>79</v>
       </c>
@@ -3754,25 +3896,25 @@
         <v>80</v>
       </c>
     </row>
-    <row r="77" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="77" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C77" s="5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="78" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="78" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C78" s="5" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="79" spans="3:27" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="80" spans="3:27" ht="19" x14ac:dyDescent="0.25">
-      <c r="C80" s="92" t="s">
+    <row r="79" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="80" spans="3:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C80" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="D80" s="93"/>
-      <c r="E80" s="94"/>
-    </row>
-    <row r="81" spans="3:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D80" s="83"/>
+      <c r="E80" s="84"/>
+    </row>
+    <row r="81" spans="3:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C81" s="9" t="s">
         <v>84</v>
       </c>
@@ -3783,17 +3925,17 @@
         <v>88</v>
       </c>
     </row>
-    <row r="83" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="83" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C83" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="84" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="84" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C84" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="85" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="85" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C85" t="s">
         <v>87</v>
       </c>
@@ -3801,31 +3943,31 @@
         <v>83</v>
       </c>
     </row>
-    <row r="87" spans="3:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="88" spans="3:10" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C88" s="92"/>
-      <c r="D88" s="93"/>
-      <c r="E88" s="94"/>
-    </row>
-    <row r="89" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="87" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="88" spans="3:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C88" s="82"/>
+      <c r="D88" s="83"/>
+      <c r="E88" s="84"/>
+    </row>
+    <row r="89" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C89" s="2"/>
       <c r="D89" s="3"/>
       <c r="E89" s="4"/>
     </row>
-    <row r="90" spans="3:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C90" s="9"/>
       <c r="D90" s="57"/>
       <c r="E90" s="11"/>
     </row>
-    <row r="94" spans="3:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="95" spans="3:10" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C95" s="92" t="s">
+    <row r="94" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="95" spans="3:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C95" s="82" t="s">
         <v>97</v>
       </c>
-      <c r="D95" s="93"/>
-      <c r="E95" s="94"/>
-    </row>
-    <row r="96" spans="3:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="D95" s="83"/>
+      <c r="E95" s="84"/>
+    </row>
+    <row r="96" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C96" s="68" t="s">
         <v>99</v>
       </c>
@@ -3837,7 +3979,7 @@
       <c r="I96" s="71"/>
       <c r="J96" s="67"/>
     </row>
-    <row r="97" spans="3:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="97" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C97" s="72" t="s">
         <v>100</v>
       </c>
@@ -3849,7 +3991,7 @@
       <c r="I97" s="74"/>
       <c r="J97" s="67"/>
     </row>
-    <row r="98" spans="3:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="98" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C98" s="75" t="s">
         <v>101</v>
       </c>
@@ -3873,7 +4015,7 @@
       </c>
       <c r="J98" s="67"/>
     </row>
-    <row r="99" spans="3:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="99" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C99" s="75">
         <v>1</v>
       </c>
@@ -3897,7 +4039,7 @@
       </c>
       <c r="J99" s="67"/>
     </row>
-    <row r="100" spans="3:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="100" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C100" s="75">
         <v>2</v>
       </c>
@@ -3921,7 +4063,7 @@
       </c>
       <c r="J100" s="67"/>
     </row>
-    <row r="101" spans="3:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="101" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C101" s="75">
         <v>3</v>
       </c>
@@ -3947,7 +4089,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="102" spans="3:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="102" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C102" s="75">
         <v>4</v>
       </c>
@@ -3971,7 +4113,7 @@
       </c>
       <c r="J102" s="67"/>
     </row>
-    <row r="103" spans="3:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="103" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C103" s="75">
         <v>5</v>
       </c>
@@ -3995,7 +4137,7 @@
       </c>
       <c r="J103" s="67"/>
     </row>
-    <row r="104" spans="3:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="104" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C104" s="77">
         <v>6</v>
       </c>
@@ -4019,7 +4161,7 @@
       </c>
       <c r="J104" s="67"/>
     </row>
-    <row r="105" spans="3:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="105" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C105" s="77">
         <v>7</v>
       </c>
@@ -4043,7 +4185,7 @@
       </c>
       <c r="J105" s="67"/>
     </row>
-    <row r="106" spans="3:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="106" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C106" s="77">
         <v>8</v>
       </c>
@@ -4067,7 +4209,7 @@
       </c>
       <c r="J106" s="67"/>
     </row>
-    <row r="107" spans="3:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="107" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C107" s="77">
         <v>9</v>
       </c>
@@ -4091,7 +4233,7 @@
       </c>
       <c r="J107" s="67"/>
     </row>
-    <row r="108" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C108" s="79">
         <v>10</v>
       </c>
@@ -4115,26 +4257,254 @@
         <v>109</v>
       </c>
     </row>
+    <row r="111" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C111" s="100" t="s">
+        <v>118</v>
+      </c>
+      <c r="D111" s="101"/>
+      <c r="E111" s="102"/>
+    </row>
+    <row r="112" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C112" s="103" t="s">
+        <v>17</v>
+      </c>
+      <c r="D112" s="104">
+        <v>0.3</v>
+      </c>
+      <c r="E112" s="105"/>
+    </row>
+    <row r="113" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C113" s="103" t="s">
+        <v>117</v>
+      </c>
+      <c r="D113" s="104">
+        <v>2.0019999999999998</v>
+      </c>
+      <c r="E113" s="105" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="114" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C114" s="103" t="s">
+        <v>113</v>
+      </c>
+      <c r="D114" s="106">
+        <f>D113/D112</f>
+        <v>6.6733333333333329</v>
+      </c>
+      <c r="E114" s="105" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="115" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C115" s="103" t="s">
+        <v>114</v>
+      </c>
+      <c r="D115" s="104">
+        <v>10</v>
+      </c>
+      <c r="E115" s="105"/>
+    </row>
+    <row r="116" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C116" s="107" t="s">
+        <v>115</v>
+      </c>
+      <c r="D116" s="108">
+        <f>D114/D115</f>
+        <v>0.66733333333333333</v>
+      </c>
+      <c r="E116" s="109" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="117" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="118" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B118" s="2"/>
+      <c r="C118" s="113" t="s">
+        <v>116</v>
+      </c>
+      <c r="D118" s="113"/>
+      <c r="E118" s="113"/>
+      <c r="F118" s="113"/>
+      <c r="G118" s="113"/>
+      <c r="H118" s="113"/>
+      <c r="I118" s="113"/>
+      <c r="J118" s="113"/>
+      <c r="K118" s="113"/>
+      <c r="L118" s="114"/>
+    </row>
+    <row r="119" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B119" s="5"/>
+      <c r="C119" s="110">
+        <v>1</v>
+      </c>
+      <c r="D119" s="110">
+        <v>2</v>
+      </c>
+      <c r="E119" s="110">
+        <v>3</v>
+      </c>
+      <c r="F119" s="110">
+        <v>4</v>
+      </c>
+      <c r="G119" s="110">
+        <v>5</v>
+      </c>
+      <c r="H119" s="110">
+        <v>6</v>
+      </c>
+      <c r="I119" s="110">
+        <v>7</v>
+      </c>
+      <c r="J119" s="110">
+        <v>8</v>
+      </c>
+      <c r="K119" s="110">
+        <v>9</v>
+      </c>
+      <c r="L119" s="111">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="120" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B120" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C120" s="104">
+        <f>$D$116*(C$119-1)+$D$116/2</f>
+        <v>0.33366666666666667</v>
+      </c>
+      <c r="D120" s="104">
+        <f t="shared" ref="D120:L120" si="1">$D$116*(D$119-1)+$D$116/2</f>
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="E120" s="104">
+        <f t="shared" si="1"/>
+        <v>1.6683333333333334</v>
+      </c>
+      <c r="F120" s="104">
+        <f t="shared" si="1"/>
+        <v>2.3356666666666666</v>
+      </c>
+      <c r="G120" s="104">
+        <f t="shared" si="1"/>
+        <v>3.0030000000000001</v>
+      </c>
+      <c r="H120" s="104">
+        <f t="shared" si="1"/>
+        <v>3.6703333333333337</v>
+      </c>
+      <c r="I120" s="104">
+        <f t="shared" si="1"/>
+        <v>4.3376666666666663</v>
+      </c>
+      <c r="J120" s="104">
+        <f t="shared" si="1"/>
+        <v>5.0049999999999999</v>
+      </c>
+      <c r="K120" s="104">
+        <f t="shared" si="1"/>
+        <v>5.6723333333333334</v>
+      </c>
+      <c r="L120" s="6">
+        <f t="shared" si="1"/>
+        <v>6.339666666666667</v>
+      </c>
+    </row>
+    <row r="121" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B121" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C121" s="104">
+        <f>$D$116*(C$119-1)</f>
+        <v>0</v>
+      </c>
+      <c r="D121" s="104">
+        <f t="shared" ref="D121:L121" si="2">$D$116*(D$119-1)</f>
+        <v>0.66733333333333333</v>
+      </c>
+      <c r="E121" s="104">
+        <f t="shared" si="2"/>
+        <v>1.3346666666666667</v>
+      </c>
+      <c r="F121" s="104">
+        <f t="shared" si="2"/>
+        <v>2.0019999999999998</v>
+      </c>
+      <c r="G121" s="104">
+        <f t="shared" si="2"/>
+        <v>2.6693333333333333</v>
+      </c>
+      <c r="H121" s="104">
+        <f t="shared" si="2"/>
+        <v>3.3366666666666669</v>
+      </c>
+      <c r="I121" s="104">
+        <f t="shared" si="2"/>
+        <v>4.0039999999999996</v>
+      </c>
+      <c r="J121" s="104">
+        <f t="shared" si="2"/>
+        <v>4.6713333333333331</v>
+      </c>
+      <c r="K121" s="104">
+        <f t="shared" si="2"/>
+        <v>5.3386666666666667</v>
+      </c>
+      <c r="L121" s="6">
+        <f t="shared" si="2"/>
+        <v>6.0060000000000002</v>
+      </c>
+    </row>
+    <row r="122" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B122" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C122" s="10">
+        <f>$D$116*(C$119)</f>
+        <v>0.66733333333333333</v>
+      </c>
+      <c r="D122" s="10">
+        <f t="shared" ref="D122:L122" si="3">$D$116*(D$119)</f>
+        <v>1.3346666666666667</v>
+      </c>
+      <c r="E122" s="10">
+        <f t="shared" si="3"/>
+        <v>2.0019999999999998</v>
+      </c>
+      <c r="F122" s="10">
+        <f t="shared" si="3"/>
+        <v>2.6693333333333333</v>
+      </c>
+      <c r="G122" s="10">
+        <f t="shared" si="3"/>
+        <v>3.3366666666666669</v>
+      </c>
+      <c r="H122" s="10">
+        <f t="shared" si="3"/>
+        <v>4.0039999999999996</v>
+      </c>
+      <c r="I122" s="10">
+        <f t="shared" si="3"/>
+        <v>4.6713333333333331</v>
+      </c>
+      <c r="J122" s="10">
+        <f t="shared" si="3"/>
+        <v>5.3386666666666667</v>
+      </c>
+      <c r="K122" s="10">
+        <f t="shared" si="3"/>
+        <v>6.0060000000000002</v>
+      </c>
+      <c r="L122" s="112">
+        <f t="shared" si="3"/>
+        <v>6.6733333333333338</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="C95:E95"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="C88:E88"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="C80:E80"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="G30:I30"/>
+  <mergeCells count="34">
+    <mergeCell ref="C118:L118"/>
+    <mergeCell ref="C111:E111"/>
     <mergeCell ref="J37:Y37"/>
     <mergeCell ref="J49:S49"/>
     <mergeCell ref="C39:C43"/>
@@ -4149,6 +4519,24 @@
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="D59:E59"/>
     <mergeCell ref="D60:E60"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="C95:E95"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="C88:E88"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="C80:E80"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="F49:I49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>